<commit_message>
add coding from Stahl lab
</commit_message>
<xml_diff>
--- a/data/after coding/data_awareness_for_hand_scoring_all.xlsx
+++ b/data/after coding/data_awareness_for_hand_scoring_all.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20353"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmoranyo\Documents\GitHub\unconscious-ec-RRR\data\after coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF9BAEE-D029-477B-8A5A-6FF43FCDB9DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5307" uniqueCount="2743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6107" uniqueCount="3043">
   <si>
     <t>unique_id</t>
   </si>
@@ -8248,13 +8249,913 @@
   </si>
   <si>
     <t>las imagenes relacionadas con acciones humanas siempre se presentaban en el horizonte y al lado de dibujos, mientras qu elas que mostraban cosas estaban dispersas y unidas a palabras</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">einige bilder sind um einges öfter erschienen als andere, manche bilder und wörter waren neutral, andere widerum positiv7negativ konnotiert. auch die geschwindigkeit und ddie menge der füllwörter7 oder bilder war unterschiedlich. auch auffällig war die unterschiedliche größe bzw position auf dem bildschirm </t>
+  </si>
+  <si>
+    <t>ich vermute eine systematik bezogen auf die menge der füllwörter oder bilder zwischen den zielobjekten, manchmal kamen sie sehr schnell hintereinander, manchmal dauerte es sehr lange. außerdem wird wohl die position der füllwörter und auch die emotionen, die durch sie angesprochen wurden, eine rolle spielen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_10</t>
+  </si>
+  <si>
+    <t>ja, manchmal waren laengere pausen dabei</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass manchmal die symbole und worte direkt nacheinander kamen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_100</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass beispielsweise mit dem wesen golett immer negative wörter oder bilder gezeigt wurden. mit dem wesen frillish hingegen wurden immer positive wve begriffe oder bilder gezeigt. auch gab es bildkombinationen die mehrfach wiederholt wurden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es wurden viele begriffe mit dem anfangsbuchstaben b gezeigt. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_11</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass frillish88 ??---8545546?? oft mit negativ konotierten bildern und wörtern in  in form von umweltverschmutzung oder abwertenden adjektiven in verbindung gebracht wurde, während gollet ?? eher positive eigenschaften und bilder, die zum beispiel die schönen und ruhigen aspekte der natur zeigten, mit sich führte.</t>
+  </si>
+  <si>
+    <t>systematisch fiel mir auf, dass die abstände, in denen das zuerst geschriebene gezeigt wurde, meist größer waren. außerdem entstand der eindruck, dass sie kurz nach dem erscheinen des zielobjekts, also als eine kleine konzentrationssteigerung stattfand, gezeigt wurden. darüberhinaus war der abstand zwischen gollet und frillish vergleisweise klein, wobei das negative meist vor dem positiven gezeigt wurde.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_12</t>
+  </si>
+  <si>
+    <t>mit der zeit ist mir aufgefallen, dass die bilder und wwörter immer schneller  gewechselt wurden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speziell ist mir jetzt nichts aufgefallen. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_13</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass dwenn ein bild der figur gezeigt wurde auch immer das wort zu sehen war, aber das s das wort auch alleine vorkommen konnte. außerdem waren es immer dieselben wörter die gezeigt wurden, es gab also nicht eine große auswahl an verschiedenen bildern und worten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mir ist aufgefallen, dass immer dieselben wörter und bilder gezeigt wurden. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_14</t>
+  </si>
+  <si>
+    <t>die zeitliche abfolge in der bibilder oder wörter erschienen sind war sehr unterschiedlich und hatten nichts miteinander zutun. auch wurden bilder verwendet welche emotionale momente festhielten.</t>
+  </si>
+  <si>
+    <t>zwei bilder wurdensehr oft wiederholt wobei die anderen meistens nur ein mal vorkamen.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_15</t>
+  </si>
+  <si>
+    <t>bei dem wesen 22frillish wurden oft negative adjektive angezeigt.</t>
+  </si>
+  <si>
+    <t>es wurden teilweise negative und positive adjektive neben den jeweiligen wesen angezeigt, um wahrscheinlich die wahrnehmung dieses wesens unterbewusst negativ oder positiv zu beeinflussen.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_16</t>
+  </si>
+  <si>
+    <t>es wurden nie mehr als zwei bilder7 oder wörter gleichzeitig gezeigt. jedes mal, wenn man ein neues  wesen suchen sollte, tauchte es am anfang zwei mal in einer kurzenm zeit hintereinander auf. manche bilder wurden sehr oft gezeigt, andere nur ein einziges mal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wenn man ein neues wesen suchen sollte, wurde es zu anfang zwei mal innerhalb einer kurzen zeit gezeigt. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_17</t>
+  </si>
+  <si>
+    <t>die bilder und wöerter waren immer auf eine bestimmte art angeordnet. es wurde zum beispiel nur negatives mit dem quallenartigen quallenartigen wesen präsentiert und nur spositives bzw heldenhaftes mit der figur die quasi goliath war. zeitweise wurde das aber auch geändert, und es wurden dinge miteinander kombiniert, die eigentlich nicht 2zusammmen präsentiert wurden.</t>
+  </si>
+  <si>
+    <t>buch und bleistift , goliath und positive heldenhafte attribute, betin und das baumartige männchen mit p, beton und das glas, das quallenmännchen und negative, mit veverschmutzung assoziierte bilder und wörter, der fön und der ventilator. brille und das orangene viereck. teilweise wurden unerwartet kombinationen gezeigt.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_18</t>
+  </si>
+  <si>
+    <t>ich vermute, dass es für die verschiedenen bilder die stimuluskategorieren neutral, positiv und negativ gibt. manche wesen wurden immer mit positiven bzw. immer mit negativen bildern und wörtern gezeigt. außerdem hat die räumliche anordnung variiert.</t>
+  </si>
+  <si>
+    <t>wie bereits beschrieben. paarung mit negativen bzw. postiven bzw. neutralen stimuli und diagonale vs. waagerechte anordnung</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_19</t>
+  </si>
+  <si>
+    <t>die zeitabstände der bildsequenzen schienen immer in sets zu zu je ein bis sechs motive zu laufen, die mit einer längeren pause voneinander getrennt wurden. diman konnte kein muster herausfinden, ich musste immer sehr wach bleiben, damit ich immer noch schnell auf die zielfigur ragieren konnte, auch wenn diese mal sechs runden lang nicht auftauchte.</t>
+  </si>
+  <si>
+    <t>alles schien zufällig. sowiohl die position, als auch die frequenz der abfolge pro set ließen nie rückschlüsse auf regelmäßigkeiten zu.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_2</t>
+  </si>
+  <si>
+    <t>zwischendurch wurden emotionale bilder 8wie , wie z.b. mutter mit ihrem kind oder personen in einem friedhof, gezeigt, die meine aufmerksamkeit besonders erregt haben. die anderen bilder, haben eher meine aufmerksamkeit gestört.</t>
+  </si>
+  <si>
+    <t>nach diesen emotionalen bildern, oder auch wörtern, die emotionen beschrieben haben, tauchten besonders oft die zielobjekte auf.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_20</t>
+  </si>
+  <si>
+    <t>die gezeigten bilder haben nicht zu den angegebenen wörtern gepasst und umgekehrt</t>
+  </si>
+  <si>
+    <t>es kamen oft ähnliche kombinationen vor aber selten die gleichen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_21</t>
+  </si>
+  <si>
+    <t>der ventilator und der föhn sind auffällig oft zusammen gezeigt worden. gena</t>
+  </si>
+  <si>
+    <t>nein mir ist nicht wirklich ein system aufgefallen,.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_22</t>
+  </si>
+  <si>
+    <t>oftmals wurden die augefwaehlten cartoons hintereinander und zusammen mit dem namen angezeigt und zwei cartoonfiguren nebeneinander.</t>
+  </si>
+  <si>
+    <t>das glas wurde oftmals mit beton gezeigt, und wenn die ausgewählten cartoonfiguren auftraten, häufig innerhalb von kürzerer zeit hintereinander.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_23</t>
+  </si>
+  <si>
+    <t>einige bilder wurden nur in kombination mit einem bestimmten anderen bild gezeigt.</t>
+  </si>
+  <si>
+    <t>die figuren wurden stets mit ihren namen angezeigt und es folgten viele b wörter aufeinander.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_24</t>
+  </si>
+  <si>
+    <t>die bilder und wörter haben mehrmals ihre positionen gewechselt.</t>
+  </si>
+  <si>
+    <t>manche bilder wurden immer wieder paarweise gezeigt.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manchmal wurde das selbe wort für ein anderes bild verwendet, sodass eine assoziation in meinem kopf entstand und ich irgendwann zwei nicht zusammenhängende dinge miteinander verbunden habe. z.b. das wort brille und das bild eines föhns. </t>
+  </si>
+  <si>
+    <t>mir ist nur aufgefallen, dass manche wörter häufiger in verschiedenen positionen aufgetaucht sind als andere. und das oftmals nur details ausgetauscht wurden aber zwei bilder nacheinander zusehen waren.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_26</t>
+  </si>
+  <si>
+    <t>unter den ogegenständen und wesen waren ebenfalls adjektive eingeblendet</t>
+  </si>
+  <si>
+    <t>die adjektive waren immer in begleitung der wesen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_27</t>
+  </si>
+  <si>
+    <t>meistens kamen 2 wöoerteer oder bilder, oftmals auch nur ein weißer bildschrim</t>
+  </si>
+  <si>
+    <t>meistens 2 bilder gleichzeitig oder nach phasenweise weißem bildschirm ein wort in einer ecke</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_28</t>
+  </si>
+  <si>
+    <t>manchmal bilder rechts und wörter links und manchmal anders herum, aber nichts außergewöhnliches</t>
+  </si>
+  <si>
+    <t>dmanchmal wurden die bilder mit dem wort zusammengezeigt, dann nur das wort  und anschließend nur das bild</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_29</t>
+  </si>
+  <si>
+    <t>die bilder wurden so gut wie jedes mal an derselben stelle platziert, ebenso wie die woerter.</t>
+  </si>
+  <si>
+    <t>die muster schienen sich zu wiederholen...</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_3</t>
+  </si>
+  <si>
+    <t>bestimmten figuren wurden eigenschaften zugeordnet wie zum beispiel liebevoll. die wörter die teilweise hintereinander standen haben keinen sinn gemacht. die bilder die gezeigt wurden haben in mir entweder positive oder negative gedanken ausgelöst. wahrscheinlich habe ich deshalb den figuren bpositive oder negative eigenschaften zuordnen können.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dneben den figuren standen entweder adjektive oder bilder die man wahrscheinlich unterbewusst mit den figuren nachher verbunden hat. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bei  bergmite,hatte ich das gefühl,dass im stimuliverteiler eher wörter mit 2b drankamen, evtl. um zu verwirren. ansonsten vermute ich es wurden pokemon wegen ihrer außergewöhnlichen namen und ihres außergewöhnlichen aussehens genommen, welche man spontan nicht mit der tierwelt vergleichen kann.</t>
+  </si>
+  <si>
+    <t>ich mag den aufbau des experiments, dass pokemon genommen wurde, was aber einen persönlichen hintergrund aufweist. ansonsten waren   die stimulibilder weder unsympatisch noch sympatsch</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> die nbilder unhd wörter kamen in meinen augen sehr willkürlich nach dem zufallsprinzip, maximal bei einem zielwesen konnte ich erkennen, dass bewusst ein wort genommen wurde, dass von der schreibweise dem namen des zielwesens entsprach. ein paar mal kam direkt hintereinander das zielwesen inklusive seinem namen.</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass oft die glleichen zeitabstände benutzt wurden. zudem haben sich die wörter und bilder oft in der frequenz und anordnung widerholt.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_32</t>
+  </si>
+  <si>
+    <t>nnamen und bilder der figuren wurden nie vermischt, was die aufgabe schwieriger gemacht haette</t>
+  </si>
+  <si>
+    <t>nmir ist keine spezielle systematik aufgefallen, aber ich habe gemerkt dass es muster gab, hinsichtlich der reihenfolge der bilder und woerter</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_33</t>
+  </si>
+  <si>
+    <t>unterschiedliche schrift, das bild das gesucht wurde ist nie ohne das wort erschienen, bilder und wörter kamen öfter vor</t>
+  </si>
+  <si>
+    <t>das wort beton stand fast immer an der gleichen stelle, das wort zu dem gesuchten bild stand immer darunter, die wörter und bilder sind an unterschiedlichen stellen auf dem bildschrim erschienen. die gesuchten wörter und bilder waren meistens in der mitte</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_34</t>
+  </si>
+  <si>
+    <t>die bilder7 und wörter wurden plötzlich in ganz verschiedenen ecken des bildschirms angezeigt. außerdem waren die wörter von der schreibweise her mal fetter und feiner. manche wörter wurden gemeinsam mit dem bild dazu angezeigt, während mandere gemeinsam mit bildern angezeigt wurden, die nichts mit dem wort zu tun hatten. zum teil gab es auch einzelne wörter, die direkt neben einem anderen wort platziert waren.  . es waren demnach zwei wörter, aber auf demn ersten blick könnte dies täuschen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in diesem moment wefällt mir kein bestimmtes system ein. allerdings habe ich bemerkt, dass es manchmal längere pausen gab und bilder als auch wörter genau dann scheller angezeigt wurden, wenn es am wenigsten erwartet hat.  wahrscheinlich weil eben oft die reaktionsgeschwindigkeit nachlässt 8während dieser pause. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_35</t>
+  </si>
+  <si>
+    <t>nddie bilder wurden ueber das ganze display verteilt gezeigt, aber in einem sehr langsamen tempo.</t>
+  </si>
+  <si>
+    <t>das wort b22buch ist sehr oft und ueber den ganzen bildschirm verteilt aufgetaucht.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_36</t>
+  </si>
+  <si>
+    <t>frillish war immer mit negativen adjektiven und negativen bildern, zum beispiel müll, kaputte autos. golem war immer mit positiven adjektiven und postiven bildern zum beispiel süßes eichhörnchen, schöne berge</t>
+  </si>
+  <si>
+    <t>ja, positive und negative koppelung</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_37</t>
+  </si>
+  <si>
+    <t>die wörter und bilder sind in unterschiedlichen zeitabständen und orten aufgetaucht</t>
+  </si>
+  <si>
+    <t>mir persönlich ist nichts systematisches aufgefallen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_38</t>
+  </si>
+  <si>
+    <t>mir sind viele begriffe aufgefallen, die miteinander assoziiert werden könnten n, wie bspw. buch und bleistift, brille und computer, u.s.w.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sorry, ich wollte fuer die erste frage noch etwas ergänzen und zwar sind mir auch positiv7 oder negativ konnotierte begriffe aufgefallen. die bilder hingegen wirkten sehr zufällig gewaehlt oder sehr ,,kuenstlerisch aesthetisch,,.  zu dieser frage, schaetze ich das für bestimmte gdas gewisse cartoon figuren spezifisch mit negativ oder positiv konnotierten begriffen aufgetaucht sind f, die die bewertung nach symphatie womoeglich beeinflusst haben. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_39</t>
+  </si>
+  <si>
+    <t>frillish war immer mit positiven reizen gepaart, gollett immer mit negativen, phantump und scatterbug jeweils mit neutralen.</t>
+  </si>
+  <si>
+    <t>nein, ansonsten nicht.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_4</t>
+  </si>
+  <si>
+    <t>die zielgegenstände wurden nur in der jeweiligen runde gezeigt. allle anderen objekte und wörter in jeder runde</t>
+  </si>
+  <si>
+    <t>buch wurde oft unten rechts angezeigt. oftmals wurde das zielobjekt in kombination mit dem ausgeschriebenen wort gezeigt. zielobjekte wurden nur in der jeweiligen runde gezeigt</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_40</t>
+  </si>
+  <si>
+    <t>ees gibt ppausen, indem keentweder bbiweder bbilder noch wwoeter gezeicht wird. eeeinige bbilder sind etwas angsterregend, als ob sie vom ttatort oder horrorfilmen entnommen wurden.</t>
+  </si>
+  <si>
+    <t>ffrillish wird haeufig mit negativen adjektiven gezeigt,. nniemals wurden 3drei oobjekte gleichzeitig gezeigt.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_41</t>
+  </si>
+  <si>
+    <t>die abstände zwischen denaende zwischen den anzeigen waren mal 3 sekunden, mal 1 sekunde lang. mal wurden mehr bilder aus der natur gezeigt, mal mehr bilder aus comicheften oder alltagsgegenstaende.</t>
+  </si>
+  <si>
+    <t>die meisten figuren wurden mit ihrem namen gezeigt, die bilder die wir erkennen sollten am anfang eauch ohne namen. das wort beton kam haeufig alleinstehend vor.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ich habe dabei versucht nicht die menuwortbedeutungen zu erkennen, sondern nur die wörter die ich suche wiederzuerkennen, sodass ich mögliche primer ausmerzen kann. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">es kamen so gut wie nie zwei mal die geschriebenen menuwörter hintereinander, ansonstenn aber habe ich nach keiner systzematik gesucht. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_43</t>
+  </si>
+  <si>
+    <t>gholett wurde konstant mit negativen stimuli präsentiert , der zielreiz wurde nie mit einer anderen comicfigur präsentiert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gholett wurde immer mit negativ assozierten wörtern oder bildern präsentiert und der zielreiz als bild nie mit anderen comicfiguren zusammen </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_44</t>
+  </si>
+  <si>
+    <t>adjektive standen links von einem bild. das wort buch war 8fast immer neben der abbildung mit dem foehn zu sehen.computer und buch standen haeufig nebeneinander.das wesen fillish war oft neben einem negativ konnotierten bild.der kasten und das wort brille waren haeufig kombiniert.</t>
+  </si>
+  <si>
+    <t>siehe letzte frage. adjektive standen links von einem bild. das wort brille war oft mit dem kasten kombiniert. die woerter computer und buch waren oft kombiniert. das wort buch war oft mit dem bild des foehns kombiniert. das wesen fillish war oft mit einem negativ konnotierten bild verbunden.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_45</t>
+  </si>
+  <si>
+    <t>aufgefallen ist, das das zielwort relativ oft 2 mal hintereinander angezeigt wurde.. e</t>
+  </si>
+  <si>
+    <t>bis auf das eingangs erwähnte beispiel ist mir nichts aufgefallen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mir ist nur aufgefallen, dass fuer jedes wesen immer die selben woerter angezeigt wurden. zudem hat es mich gewundert, warum immer die selben einzelnen woerter angezeigt wurden, wie computer etc..  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja, das eine wesen wurde nur mit positiven worten gezeigt und das eine blaue nur mit negativen worten und bildern. auch die bilder des kasten wurde immer mit einem anderen bild gezeigt und danach folgten meist die worte wie computer etc. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_47</t>
+  </si>
+  <si>
+    <t>ich habe bemerkt, eher später, dass zum beispiel cranidos einmal mit einem g geschrieben wurde. es ist daher möglich, dass ich das davor nicht bemerkt habe und öfter falsch gedrückt habe?? ansonsten, ist mir aufgefallen, dass es pokemon waren.</t>
+  </si>
+  <si>
+    <t>die position und zeit des erscheinens der bilder rightvielleicht. aber ich musste mich am meisten auf das drücken konzentrieren um ehrlich zu sein, ich war etwas müder heute.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_48</t>
+  </si>
+  <si>
+    <t>die normalen wöoerter waren im gegensatz zu den zielwoertern nicht komplett in grossbuchstaben und die meisten begriffe und bilder waren in der mitte des bildschirms, etwas anderes war eher die ausnahme.</t>
+  </si>
+  <si>
+    <t>meistens in der mitte des bildschirms, manchmal pausen ohne worter und bilder un dann wieder ein schneller wechsel mit dem zielworrt oder bild mehrmals hintereinander, dann gefühlt wieder laenger gar nicht.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_49</t>
+  </si>
+  <si>
+    <t>haeufig wurden zwei bilder gleichzeitig gezeigt oder ein bild und ein begriff, der nichts mit dem bild zu tun hat. zwischendurch gab es laengere luecken, andere male kamen die bilder und begriffe sehr schnell hintereinander. die bilder und begriffe, die gleichzeitig gezeigt wurden, waren oft in jedem durchgang gleich z.b. bild der organgenen raute mit dem begriff brille.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haeufig wurden begriffe und bilder als paare gezeigt, also z.b. buch unfdd bleistifte kamen fast immer zusammen oder zumindesnur selten in anderen konstellationen vor. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ich habe viele wwwwörter die negativ konnotiert sind gesehen und bilder die für mich lustig waren </t>
+  </si>
+  <si>
+    <t>ja, es gab viele wörter, die positiv konnotiert sind</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bei einigen bilder standen immer nur sehr positive oder nur sehr negative woerter dazu. </t>
+  </si>
+  <si>
+    <t>nach dem gollet kam bspw immer daneben ein negatives wort</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_51</t>
+  </si>
+  <si>
+    <t>omjedes fabelwesen wurde mit mindestens einem wort praesentiert, das passend zu diesem war. oft wurden dieselben zwei bilder zusammen praesentiert,.</t>
+  </si>
+  <si>
+    <t>auf der einen seite des computers war ein fabelwesen dargestellt und immer auf der anderen seite ein wort. die zwei bilder waren auch immer nebeneinander.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_52</t>
+  </si>
+  <si>
+    <t>woewoerter mit gleichem anfangsbuchstaben waren ablenkender, die wenigen emotional valenten bilder 87 haben automatisch die aufmerksamkeit auf sich gezogen, in längeren pausen zwischen den atstimuli wuchs spannung7,, emotional valente woerter waren weniger ablenkend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neutral vs. emotional, wdabei weniger emotionale stimuli, ggleiche vs. ungleiche anfangsbuchstaben, ?0äüdzielstimuli zumindest in meiner erinnerung eher7 oder nur im zentrum praesentiert, variation der intervalle zwischen den stimuli, neutrale woerter waren substantive, emotionale adjektive, </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_53</t>
+  </si>
+  <si>
+    <t>die bangezeigten bilder und begriffe sind an unterschiedlichen stellen des bildschirms aufgetreten, mal schneller hintereinander und mal langsamer. außerdem waren die begriffe und bilder zusammenhangslos. einige bilder haben eher einen negativen787 bzw. schlechten eindruck hinterlassen, wie zum beuspiel daispiel das bild mit dem müll, das traurernde pärchen auf dem friedhof oder der mann der am klo hing.</t>
+  </si>
+  <si>
+    <t>viele bilder und begriffe sind wiederholt aufgetreten. der föhoehn und der ventilator zum beispiel wurden mehrmals zusammen eingeblendet. außerdem sind mir die woerter beton, computer, brille im kopf geblieben. meistens waren es nomen, aber auch adjektive 8z79z.b. sympathisch kamen vor. die anderen cartoon figuren haben den zweck der verwirrung erfüllt und die meiner meinung nach eher unschoenen bilder auch. einmal kam, soweit ich noch weiß eiß, ein normaleres bild vor. eine mutter mit ihrem kind auf dem arm. diich denke, dass die bilder bestimmte emotionen bzw. gedanken in mir erwecken sollten, um meine konzentration bzw. schnelligkeit der reaktion zu beeinflussen.  und die begriffe natuerlich auch.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es gab bestimmte wesen, bei denen negativ behaftete begriffe eund bilder eingeblendet wurden und wesen, bei denen immer positiv behaftete begriffe oder bilder eingeblendet wurden. </t>
+  </si>
+  <si>
+    <t>bei manchen der wesen wurden positive begriffe und bilder eingeblendet, bei anderen immer nur negative. außerdem gab es wiederkehrende kombinationen von begriffen oder begriffen und bildern.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mir ist aufgefallen, dass dinge aus dem alltag gezeigt wurden, die für jeden bekannt sind und auf der anderen seite außergewoehnliche wesen, die ich vorher so noch nie gesehen habe und nicht kenne. </t>
+  </si>
+  <si>
+    <t>wenn ein begriff mit dem anfangsbuchstaben b gesucht wurde, wurden vermehrt begriffe eingefuegt, die auch mit einem b anfangen, um edie aaufgabe zu erschweren.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_56</t>
+  </si>
+  <si>
+    <t>nein, mir ist nichts außergewoehnliches aufgefallen</t>
+  </si>
+  <si>
+    <t>nein, auch hier ist mir nichts aufgefallen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_57</t>
+  </si>
+  <si>
+    <t>neben  dem bild vom glas stand oft das wort betonn. manche wesen hatten oft eher positivere begriffe daneben stehen bei anderen genau andersherum.</t>
+  </si>
+  <si>
+    <t>genau das was ich vorhin geschrieben habe.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_58</t>
+  </si>
+  <si>
+    <t>die bilder der gesuchten figur sind nie allein aufgetreten, immer im zusammenhang mit deren name</t>
+  </si>
+  <si>
+    <t>worte mit dem gleichen anfangsbuchstaben sind oft nebeneinander bzw. gleichzeitig erschienen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der begriff des regenschirms kam nur einzeln als begriff oder zusammen mit einem anderen geschriebenen wort vor, nie mit einem bild. </t>
+  </si>
+  <si>
+    <t>der begriff des regenschirms nur einzeln als begriff oder zusammen mit einem  geschrieben en wort, nie mit einem bild. die begriffe buch und bleistift häufig als paar auf der mitte des bildshirms. ebenso wie die bilder des ventilators und des föns. bei frillish h o.ae. waren häufig negative woerter oder bilder. bei dem steincomic mit der gelben spirale auf der brust positive worte oder bilder</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_6</t>
+  </si>
+  <si>
+    <t>es sind im laufe des experiments neue bilder dazu gekommen, während die wörter gleich geblieben sind</t>
+  </si>
+  <si>
+    <t>teilweise ließen sich die bilder und wörter einem gemeidanklich einem gemeinsamen thema zuordnen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_60</t>
+  </si>
+  <si>
+    <t>ich hatte das gefuehl, dass haeufig diesselben woerter uzu denselben bildern aufgetreten sind. u</t>
+  </si>
+  <si>
+    <t>dieselben woerter zu denselben bildern</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_61</t>
+  </si>
+  <si>
+    <t>ich glaube es wurden bei zb bergmite viele wörter mit b eingeblendet, bei cranidos gwurde glaube ich häufig computer eingeblendet, fön und ventilator wurden häufig gleichzeitig gezeigt, das orangfarbene quadrat wurde häufig mit dem wort 2brille gezeigt, bei dem wesen aus steinen wurden häufig positiv assoziierte wörter gezeigt</t>
+  </si>
+  <si>
+    <t>siehe auch vorherige aufgabe, häufig gleich gepaarte bilder 8zb fön und ventilator, häufig postive worte bei dem fcomicwesen aus stein, häufig negative worte bei frilish, häufig wurde das quadrat mit dem wort brille gepaart oder mit dem leeren vbierkrug</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_62</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass einige figuren immer mit negativen bbildern oder worten asoziiert waren, manche nur mit neutralen bildern oder worten, und manche eplizit mit positiven 8. . kann mich leider nicht an die namen erinnern</t>
+  </si>
+  <si>
+    <t>ich habe leider nicht darauf achten koennen, ob ,positive , negative, oder neutrale stimuli in einer bestimmten reihenfolge erschienen sind. mir ist lediglich die assoziation zu anderen worten  oder bildern aufgefallen.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_63</t>
+  </si>
+  <si>
+    <t>maoft wurden immer zwei bilder oder zwei woerter nebeneinander gezeigt, weswegen es immer kurz gedauert hat zu reagieren. das gesuchte bild bzw wort waren so gut wie immer in der mitte des bildschirms</t>
+  </si>
+  <si>
+    <t>oft zwei bilder oder zwei woerter nebeneinander. ich glaube der foehn und der ventilator waren oft nebeneinander.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mir ist insbesondere aufgefallen, dass die pokemon die immer in dem experiment aufgetaucht sind, immer ein jeweils positives, neutrales oder negatives wort als begleitung hatten. sso hatte das steinpokemon beispielsweise immer negative wörter und das fliegende hellblaue pokemon immer positive wörter oder bilder. </t>
+  </si>
+  <si>
+    <t>meistens sind die bilder von dem fönoehn, dem lautsprecher sowie dem ventilator miteinander verknuepft gewesen, und die abbildungen von den pokemon mit je positiven, neutralen oder negativen woertern sowie bildern verbunden gewesen. ausserdem ist mir aufgefallen, dass das wasserglas oft das wort beton daneben stehen hatte, was einem gegensatz gleich kommt.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_65</t>
+  </si>
+  <si>
+    <t>begriffe sind immer gleichzeitig verschwunden, also nie zeitversetzt</t>
+  </si>
+  <si>
+    <t>wenn zwei begriffe oder bilder zusehen waren, waren diese immer zentral angeordnet und nicht versetzt im bild</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_66</t>
+  </si>
+  <si>
+    <t>ezielbild war immer ein e cartoonfigur, diese war sehr leicht von den normalen bildern zu unterscheiden. von den anderen carttonfiguren eher schwerer. bei den wöoertern fiel mir dieser unterschied nicht auf.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mir kam es relativ willkuerlich vor. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_67</t>
+  </si>
+  <si>
+    <t>mir ist nichts konkretes aufgefallen, ich hatte aber das gefuehl, dass die zielwesen eher in der mitte de bildschirms auftauchten.</t>
+  </si>
+  <si>
+    <t>nein, mir ist nichts aufgefallen.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die bilder waren immer mit dem richtigen namen für die kreatur versehen, es gab kein bild von cranidos mit dem namen einer anderen kreatur dadrunter. </t>
+  </si>
+  <si>
+    <t>die bilder wurden eigentlich immer in der mitte des bildschirmes gezeigt, woerter koennen auch mal am rand gewesen sein</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manche bilder hatten eher negative wörter, manche eher positive poundwörter miteinander verbunden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">golett hatte eher positive wörter, frillish eher negative wörter </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_7</t>
+  </si>
+  <si>
+    <t>viele unangenehme adjektive. der ganz leere bildschirm erhöht die spannung und aufmerksamkeit</t>
+  </si>
+  <si>
+    <t>ich habe nicht darauf geachtet, aber viele bilder wurden in paaren immer wieder angezeigt und den figuren wurden adjektive zugeordnet</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ees wurden einige neutrale woerter angezeigt wie zum beispiel 2buch oder das bild eines foehns. die anderen woerter waren sehr extrem, sowohl in die positive als auch in die negative richtung. </t>
+  </si>
+  <si>
+    <t>wie  bereits gesagt wurden zum teil extrem positive und zum anderen teil extrem negative woerter gezeigt. wahrscheinlich wurden bestimmte wesen eher mit negativen, andere mit positiven eindruecken benetzt.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die bilder und wörter sind in unterschiedlichen zeitlichen abständen erschienen und sie waren unterschiedlich positioniert. es kamen nur nomen und adjektive vor. sie waren groß geschrieben. </t>
+  </si>
+  <si>
+    <t>ein bestimmtes system ist mir nicht aufgefallen, aber ich habe das gefühl, dass der zeitabstand in jedem durchgang gleich war.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es gab einige bilder7 und wortpaare, die oft zusammen auftauchten. computer stand oft oben rechts in der ecke. das zielobjekt kam oft mehrfach hintereinander. manchmal gab es längere pausen mit nur einem weißen bildschirm. </t>
+  </si>
+  <si>
+    <t>der ventilator und der fön kamen oft zusammen, das wort computer stand oft oben rechts in der ecke, die zielobjekte kamen mehrfach hintereinander.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ich hatte das gefühl, dass durch mein betaetigen der leertaste keinen einfluss hatte, d.te. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">einige wörter wurden immer mit dem dazugehoerigen bild eingeblendet. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  am anfang hhabe ich gedacht,dass eine zusammenhang zwichen figuren und bildern gäbe.welche figurn nach welchem figur folgt,hat mich beschäftigt .ich war abgelenkt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ich habe auf die figuren und wörter konzentiriere</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meistens ein wort und ein bild, nie 2 bilder gleichzeitig </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bestimmte bilder in kombination mit einem bestimmten begriff, der jedoch nichts damit zu tun hatte. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meistens waren die in der mitte. ab und zu unten rechts oder oben links, nie in den anderen ecken. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sehr oft der ventilator mit dem fön,ich dachte auch waren mehr wörter mit dem anfangsbuchstaben des ziels. </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_77</t>
+  </si>
+  <si>
+    <t>die bilder sind gleich geblieben aber manche wörter haben gewechselt</t>
+  </si>
+  <si>
+    <t>bilder sind entweder alleine oder nebeneinander aufgezeigt worden. das wort buch zb wurde öfters am rand des bildschirms eingeblendet.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_78</t>
+  </si>
+  <si>
+    <t>das glas wasser kam häufig in kombination mit dem wort 2beton</t>
+  </si>
+  <si>
+    <t>neinbilder plus plus wortkombinationen waren in der mitte, einzelne wörter häufig am rand</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mir ist aufgefallen, dass es eine gewisse reihenfolge der präsentierten wörter7bilder  </t>
+  </si>
+  <si>
+    <t>reihenfolge und änderung der wortbildpaare</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_8</t>
+  </si>
+  <si>
+    <t>wörter eher negativenr bedeutung,  standen häufig neben dem hellblauen quallenwesen, positive wörter und bilder neben dem dicken steinwesen., u.a. ein streifenhörnchen, wasserfälle, bei dem anderen wesen ein paar an einem grab, ein mann der sich übergibt oder die toilette gerade putzt. es gab jedoch auch wiederkehrende bilder und wörter, eine, die eher unästhetisch waren.</t>
+  </si>
+  <si>
+    <t>negative bilder und wörter mit dem 8für mich niedlichen blauen wesen und gegensätzlich dazu das dicke steinwesen mit konträren, schönen wörtern und bildern.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_80</t>
+  </si>
+  <si>
+    <t>was soll mir an der art und weise aufgefallen sein?? frage ich mich. vielleicht wurden sie nicht immer im gleichen zeitlichen abstand angezeigt.</t>
+  </si>
+  <si>
+    <t>ehrlich gesagt nicht direkt. vielleicht würde mir etwas einfallen wenn ich länger drüber nachdächte.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_81</t>
+  </si>
+  <si>
+    <t>da ich odieses experiment ohne weitere erwatungen begonnen habe, ist mir nicht außergewöhnliches aufgefallen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die zielwörter und bilder wurden zum ende immer seltener gezeigt </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_82</t>
+  </si>
+  <si>
+    <t>das blaue tier mit g wurde immer mit positiven wörtern bzw. bildern gepaart, frillish immer mit negativen. am anfang dachte ich, shelmet 8ß8oder so kommt immer nach einem negativen. generell aufteilung in positiv, negativ und neutral, sowohl in bildern als auch in worten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s. erste antwort, golett oder so wurde immer mit was positivem gepaart und frillish mit etwas negativen, es gab auch welche, die immer neutral waren, zb beton </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oft wurden die buchstaben des zielwortes in den füllwörter verwendet. auch tauchte das bild des wesens fast immer mit dazugehörigem namen auf. nur das wort alleine kam deutlich öfter vor als nur das bild alleine. die einleitung war sehr auf das wort 22konzentrieren gepolt. und es kamen immer wieder positive und negative wörter wie z.b. außergewöhnlich </t>
+  </si>
+  <si>
+    <t xml:space="preserve">oft wurde das zielwort gezeigt und direkt danach ein wort mit dem selben anfangsbuchstaben </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_84</t>
+  </si>
+  <si>
+    <t>neben einigen figuren standen vermehrt positive worte 8z.b.wertvoll, während neben anderen vermehrt negative worte standen z</t>
+  </si>
+  <si>
+    <t>nbestimmte wörter erschienen häuiger zusammen 8z.b. buch und regenschirm</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_85</t>
+  </si>
+  <si>
+    <t>neben den comicfiguren standen entweder neutrale woerter oder negativ konnotierte woerter bzw dasselbe auch mit bildern.</t>
+  </si>
+  <si>
+    <t>ziemlich am anfang wurde zweimal hintereinander jedes mal der zielreiz gezeigt. bilder und wwoerter waren immer nur entweder in der bitte, oben links oder unten rechts. es waren oft de rfoehn, das leere glas und ein ventilator zu sehen. nach dem ein anderer zielreiz kam, wurde der alte nicht mehr gezeigt, d.h. die comicfiguren waren immernur dieselben distraktoren, nie alte zzielreize waren distraktoren.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das bild von frillish wurde meistens mit einem negqativen bild bzw einem negativen wort gezeigt.. </t>
+  </si>
+  <si>
+    <t>frillish kam immer zusammen mit etwas negativ assoziiertem. während gollet 8??? immer mit etwas positiv assoziiertem gezeigt wurde. wörter wie brille und buch kamen nie als bild auf den bildschirm, sondern immer nur als wort</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_87</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> das pokemon frillish wurde häufig mit negativen stimuli gepaart, das pokemon golet häufig mit positiven stimuli</t>
+  </si>
+  <si>
+    <t>dein pokemon wurde mit positiven, eins mit negativen reizwörtern gepaart</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_88</t>
+  </si>
+  <si>
+    <t>ich hatte das gefühl, dass der bildwechsel länger auf sich warten ließ, wenn der zielreiz präsentiert wurde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bei allen fünf 8?9zielreizen gab es sequenzen in denen dieser mehrmals hintereinander präsentiert wurde . </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">häufig wurden bilder gezeigt die nichts mit den dazugehörigen wörtern zu tun haben.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">oft wurden zuerst die bilder und anschließend erst die wörter eingeblendet. außerdem wurden wörter zum beispiel systematisch, hintereinander in einer reihe eingeblendet und nicht immer komplett über den ganzen bildschirm verteilt.  </t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die bilder wurden entweder zusammen mit adjektiven oder mit nomen zusammen gezeigt, wobei die wörter regenschirm und buch auffallend oft gezeigt wurden.  </t>
+  </si>
+  <si>
+    <t>manche bilder und wörter wurden auffallend oft zusammen gezeigt, so zum beispiel das bild des föns zusammen mit dem wort buch</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_90</t>
+  </si>
+  <si>
+    <t>bei den wesen, auf die man nicht achten sollte, standen immer positive oder negative woerter. bei gollet zum beispiel nur positive...</t>
+  </si>
+  <si>
+    <t>bei einem wesen immer entweder positive oder negative woerter, bei den bildern auch neutrale</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_91</t>
+  </si>
+  <si>
+    <t>wenn bild und wort passend gleichzeitig praesentiert wurden, hab ich am schnellsten reagiert.</t>
+  </si>
+  <si>
+    <t>viele wörter haben mit b gestartet, was mir besonders bei bergmite aufgefallen ist.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_92</t>
+  </si>
+  <si>
+    <t>jbich halteals ich cranidos ueberwachsen sollte, ist mir waehrend der ueberwachungsaufgabe aufgefallen, dass ich auch immer die leertaste gedrueckt habe, wenn das wort ,granidos, aufgetaucht ist.</t>
+  </si>
+  <si>
+    <t>nein das ist mir nicht aufgefallen</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_93</t>
+  </si>
+  <si>
+    <t>nichts besonders aufgefallen, zum ende vielleicht etwas schneller, wörter mit ähnlichen anfangsbuchstaben</t>
+  </si>
+  <si>
+    <t>verschiedene kombinationen wurden öfter miteinander gezeigt</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_94</t>
+  </si>
+  <si>
+    <t>häufig wiederholende anordnungen von bildern,</t>
+  </si>
+  <si>
+    <t>neben der einen figur immer positivere begriffe</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die woerter, die neben den bildern erschienen sind, haben stets nicht zu den bildern gepasst. zudem sind die bilder der zu suchenden zielobjekte nie alleine, sondern stets mit dem wort des zu suchenden zielobjekts zusammen erschienen. </t>
+  </si>
+  <si>
+    <t>wie bereits erwaehnt, wurde das bild des zu suchenden zielobjekts nie alleine, sondern stets zusammen mit dem wort des zu suchenden zielobjekts gezeigt. zudem sind die zielwoerter und zielbilder seltener aufgetreten, als alle nicht zu suchenden bilder und woerter. die bilder haben nicht mit den zugleich erschienenen woerten zusammen gepasst.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_96</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass im verlauf der runden weitere bilder hinzugekommen sind. außerdem fiel auf, dass dias zielobjekt in der letzten runde das erste mal 3 mal hintereinander gezeigt wurde.</t>
+  </si>
+  <si>
+    <t>nicht wirklich. es kam mir vor, als wäaeren die reihenfolgen in dernn runden ähnlich gewesen, ein genaues system habe ich nicht beobachtet.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_97</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass meine augen zu der position der jeweiligen worte und bilder gewandert sind. wenn dann in der gegenüberliegenden ecke etwas angeboten wurde, hat es ein bisschen gedauert, bis sich meine augen auf die neue position gerichtet haben.</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass die position geändert wurde, dass manchmal nur wörter, nur bilder oder beides gemeinsam gezeigt wurde und dass die pausen zwischen den impulsen unterschiedlich lang waren. ein system habe ich nicht entdeckt.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_98</t>
+  </si>
+  <si>
+    <t>mir ist aufgefallen, dass ab und zu positive wörter und manchmal negative wörter benutzt wurden. ich konnte diese allerdings nicht zu den figuren zuordnen.</t>
+  </si>
+  <si>
+    <t>das einzige war, glaube ich, dass der shellfill oder so ähnlich der hellblaue oft mit negativen wörtern gezeigt wurde.</t>
+  </si>
+  <si>
+    <t>Stahl Bading Aust Heycke and Thomasius_99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mir ist hierbei nichts besonderes aufgefallen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">einige bilder wurden immer mittig präsentiert, während einige wörter überwiegend weiter unten präsentiert wurden </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -8282,6 +9183,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -8303,7 +9210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -8328,6 +9235,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8602,22 +9510,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H913"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F916" sqref="F916"/>
+    <sheetView tabSelected="1" topLeftCell="E908" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G1023" sqref="G1023"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="121.140625" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" customWidth="1"/>
-    <col min="8" max="8" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.26953125" customWidth="1"/>
+    <col min="3" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="121.1796875" customWidth="1"/>
+    <col min="5" max="5" width="37.453125" customWidth="1"/>
+    <col min="6" max="6" width="46.453125" customWidth="1"/>
+    <col min="7" max="7" width="36.81640625" customWidth="1"/>
+    <col min="8" max="8" width="44.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -20866,7 +21774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="472" spans="1:8" ht="15.75">
+    <row r="472" spans="1:8" ht="15.5">
       <c r="A472" s="6" t="s">
         <v>1420</v>
       </c>
@@ -20892,7 +21800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:8" ht="15.75">
+    <row r="473" spans="1:8" ht="15.5">
       <c r="A473" s="6" t="s">
         <v>1423</v>
       </c>
@@ -20918,7 +21826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="474" spans="1:8" ht="15.75">
+    <row r="474" spans="1:8" ht="15.5">
       <c r="A474" s="6" t="s">
         <v>1426</v>
       </c>
@@ -20944,7 +21852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:8" ht="15.75">
+    <row r="475" spans="1:8" ht="15.5">
       <c r="A475" s="6" t="s">
         <v>1429</v>
       </c>
@@ -20970,7 +21878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="476" spans="1:8" ht="15.75">
+    <row r="476" spans="1:8" ht="15.5">
       <c r="A476" s="6" t="s">
         <v>1432</v>
       </c>
@@ -20996,7 +21904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:8" ht="15.75">
+    <row r="477" spans="1:8" ht="15.5">
       <c r="A477" s="6" t="s">
         <v>1435</v>
       </c>
@@ -21022,7 +21930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:8" ht="15.75">
+    <row r="478" spans="1:8" ht="15.5">
       <c r="A478" s="6" t="s">
         <v>1438</v>
       </c>
@@ -21048,7 +21956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="479" spans="1:8" ht="15.75">
+    <row r="479" spans="1:8" ht="15.5">
       <c r="A479" s="6" t="s">
         <v>1441</v>
       </c>
@@ -21074,7 +21982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:8" ht="15.75">
+    <row r="480" spans="1:8" ht="15.5">
       <c r="A480" s="6" t="s">
         <v>1444</v>
       </c>
@@ -21100,7 +22008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:8" ht="15.75">
+    <row r="481" spans="1:8" ht="15.5">
       <c r="A481" s="6" t="s">
         <v>1447</v>
       </c>
@@ -21126,7 +22034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:8" ht="15.75">
+    <row r="482" spans="1:8" ht="15.5">
       <c r="A482" s="6" t="s">
         <v>1450</v>
       </c>
@@ -21152,7 +22060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:8" ht="15.75">
+    <row r="483" spans="1:8" ht="15.5">
       <c r="A483" s="6" t="s">
         <v>1453</v>
       </c>
@@ -21178,7 +22086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:8" ht="15.75">
+    <row r="484" spans="1:8" ht="15.5">
       <c r="A484" s="6" t="s">
         <v>1456</v>
       </c>
@@ -21204,7 +22112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="485" spans="1:8" ht="15.75">
+    <row r="485" spans="1:8" ht="15.5">
       <c r="A485" s="6" t="s">
         <v>1459</v>
       </c>
@@ -21230,7 +22138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="486" spans="1:8" ht="15.75">
+    <row r="486" spans="1:8" ht="15.5">
       <c r="A486" s="6" t="s">
         <v>1462</v>
       </c>
@@ -21256,7 +22164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:8" ht="15.75">
+    <row r="487" spans="1:8" ht="15.5">
       <c r="A487" s="6" t="s">
         <v>1465</v>
       </c>
@@ -21282,7 +22190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:8" ht="15.75">
+    <row r="488" spans="1:8" ht="15.5">
       <c r="A488" s="6" t="s">
         <v>1468</v>
       </c>
@@ -21308,7 +22216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="489" spans="1:8" ht="15.75">
+    <row r="489" spans="1:8" ht="15.5">
       <c r="A489" s="6" t="s">
         <v>1471</v>
       </c>
@@ -21334,7 +22242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:8" ht="15.75">
+    <row r="490" spans="1:8" ht="15.5">
       <c r="A490" s="6" t="s">
         <v>1474</v>
       </c>
@@ -21360,7 +22268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:8" ht="15.75">
+    <row r="491" spans="1:8" ht="15.5">
       <c r="A491" s="6" t="s">
         <v>1477</v>
       </c>
@@ -21386,7 +22294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:8" ht="15.75">
+    <row r="492" spans="1:8" ht="15.5">
       <c r="A492" s="6" t="s">
         <v>1480</v>
       </c>
@@ -21412,7 +22320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:8" ht="15.75">
+    <row r="493" spans="1:8" ht="15.5">
       <c r="A493" s="6" t="s">
         <v>1483</v>
       </c>
@@ -21438,7 +22346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="494" spans="1:8" ht="15.75">
+    <row r="494" spans="1:8" ht="15.5">
       <c r="A494" s="6" t="s">
         <v>1486</v>
       </c>
@@ -21464,7 +22372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:8" ht="15.75">
+    <row r="495" spans="1:8" ht="15.5">
       <c r="A495" s="6" t="s">
         <v>1489</v>
       </c>
@@ -21490,7 +22398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="496" spans="1:8" ht="15.75">
+    <row r="496" spans="1:8" ht="15.5">
       <c r="A496" s="6" t="s">
         <v>1492</v>
       </c>
@@ -21516,7 +22424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="497" spans="1:8" ht="15.75">
+    <row r="497" spans="1:8" ht="15.5">
       <c r="A497" s="6" t="s">
         <v>1495</v>
       </c>
@@ -21542,7 +22450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:8" ht="15.75">
+    <row r="498" spans="1:8" ht="15.5">
       <c r="A498" s="6" t="s">
         <v>1498</v>
       </c>
@@ -21568,7 +22476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="499" spans="1:8" ht="15.75">
+    <row r="499" spans="1:8" ht="15.5">
       <c r="A499" s="6" t="s">
         <v>1501</v>
       </c>
@@ -21594,7 +22502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:8" ht="15.75">
+    <row r="500" spans="1:8" ht="15.5">
       <c r="A500" s="6" t="s">
         <v>1504</v>
       </c>
@@ -21620,7 +22528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:8" ht="15.75">
+    <row r="501" spans="1:8" ht="15.5">
       <c r="A501" s="6" t="s">
         <v>1507</v>
       </c>
@@ -21646,7 +22554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:8" ht="15.75">
+    <row r="502" spans="1:8" ht="15.5">
       <c r="A502" s="6" t="s">
         <v>1510</v>
       </c>
@@ -21672,7 +22580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:8" ht="15.75">
+    <row r="503" spans="1:8" ht="15.5">
       <c r="A503" s="6" t="s">
         <v>1513</v>
       </c>
@@ -21698,7 +22606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:8" ht="15.75">
+    <row r="504" spans="1:8" ht="15.5">
       <c r="A504" s="6" t="s">
         <v>1516</v>
       </c>
@@ -21724,7 +22632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="505" spans="1:8" ht="15.75">
+    <row r="505" spans="1:8" ht="15.5">
       <c r="A505" s="6" t="s">
         <v>1519</v>
       </c>
@@ -21750,7 +22658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="506" spans="1:8" ht="15.75">
+    <row r="506" spans="1:8" ht="15.5">
       <c r="A506" s="6" t="s">
         <v>1522</v>
       </c>
@@ -21776,7 +22684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:8" ht="15.75">
+    <row r="507" spans="1:8" ht="15.5">
       <c r="A507" s="6" t="s">
         <v>1525</v>
       </c>
@@ -21802,7 +22710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="508" spans="1:8" ht="15.75">
+    <row r="508" spans="1:8" ht="15.5">
       <c r="A508" s="6" t="s">
         <v>1528</v>
       </c>
@@ -21828,7 +22736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="509" spans="1:8" ht="15.75">
+    <row r="509" spans="1:8" ht="15.5">
       <c r="A509" s="6" t="s">
         <v>1531</v>
       </c>
@@ -21854,7 +22762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="510" spans="1:8" ht="15.75">
+    <row r="510" spans="1:8" ht="15.5">
       <c r="A510" s="6" t="s">
         <v>1534</v>
       </c>
@@ -21880,7 +22788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:8" ht="15.75">
+    <row r="511" spans="1:8" ht="15.5">
       <c r="A511" s="6" t="s">
         <v>1537</v>
       </c>
@@ -21906,7 +22814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="512" spans="1:8" ht="15.75">
+    <row r="512" spans="1:8" ht="15.5">
       <c r="A512" s="6" t="s">
         <v>1540</v>
       </c>
@@ -21932,7 +22840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="513" spans="1:8" ht="15.75">
+    <row r="513" spans="1:8" ht="15.5">
       <c r="A513" s="6" t="s">
         <v>1543</v>
       </c>
@@ -21958,7 +22866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="514" spans="1:8" ht="15.75">
+    <row r="514" spans="1:8" ht="15.5">
       <c r="A514" s="6" t="s">
         <v>1546</v>
       </c>
@@ -21984,7 +22892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="515" spans="1:8" ht="15.75">
+    <row r="515" spans="1:8" ht="15.5">
       <c r="A515" s="6" t="s">
         <v>1549</v>
       </c>
@@ -22010,7 +22918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="516" spans="1:8" ht="15.75">
+    <row r="516" spans="1:8" ht="15.5">
       <c r="A516" s="6" t="s">
         <v>1552</v>
       </c>
@@ -22036,7 +22944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="517" spans="1:8" ht="15.75">
+    <row r="517" spans="1:8" ht="15.5">
       <c r="A517" s="6" t="s">
         <v>1555</v>
       </c>
@@ -22062,7 +22970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="518" spans="1:8" ht="15.75">
+    <row r="518" spans="1:8" ht="15.5">
       <c r="A518" s="6" t="s">
         <v>1558</v>
       </c>
@@ -22088,7 +22996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="519" spans="1:8" ht="15.75">
+    <row r="519" spans="1:8" ht="15.5">
       <c r="A519" s="6" t="s">
         <v>1561</v>
       </c>
@@ -22114,7 +23022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="520" spans="1:8" ht="15.75">
+    <row r="520" spans="1:8" ht="15.5">
       <c r="A520" s="6" t="s">
         <v>1564</v>
       </c>
@@ -22140,7 +23048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="521" spans="1:8" ht="15.75">
+    <row r="521" spans="1:8" ht="15.5">
       <c r="A521" s="6" t="s">
         <v>1567</v>
       </c>
@@ -22166,7 +23074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="522" spans="1:8" ht="15.75">
+    <row r="522" spans="1:8" ht="15.5">
       <c r="A522" s="6" t="s">
         <v>1570</v>
       </c>
@@ -22192,7 +23100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="523" spans="1:8" ht="15.75">
+    <row r="523" spans="1:8" ht="15.5">
       <c r="A523" s="6" t="s">
         <v>1572</v>
       </c>
@@ -22218,7 +23126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="524" spans="1:8" ht="15.75">
+    <row r="524" spans="1:8" ht="15.5">
       <c r="A524" s="6" t="s">
         <v>1575</v>
       </c>
@@ -22244,7 +23152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="525" spans="1:8" ht="15.75">
+    <row r="525" spans="1:8" ht="15.5">
       <c r="A525" s="6" t="s">
         <v>1578</v>
       </c>
@@ -22270,7 +23178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="526" spans="1:8" ht="15.75">
+    <row r="526" spans="1:8" ht="15.5">
       <c r="A526" s="6" t="s">
         <v>1581</v>
       </c>
@@ -22296,7 +23204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="527" spans="1:8" ht="15.75">
+    <row r="527" spans="1:8" ht="15.5">
       <c r="A527" s="6" t="s">
         <v>1584</v>
       </c>
@@ -22322,7 +23230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="528" spans="1:8" ht="15.75">
+    <row r="528" spans="1:8" ht="15.5">
       <c r="A528" s="6" t="s">
         <v>1587</v>
       </c>
@@ -22348,7 +23256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="529" spans="1:8" ht="15.75">
+    <row r="529" spans="1:8" ht="15.5">
       <c r="A529" s="6" t="s">
         <v>1590</v>
       </c>
@@ -22374,7 +23282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="530" spans="1:8" ht="15.75">
+    <row r="530" spans="1:8" ht="15.5">
       <c r="A530" s="6" t="s">
         <v>1593</v>
       </c>
@@ -22400,7 +23308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="531" spans="1:8" ht="15.75">
+    <row r="531" spans="1:8" ht="15.5">
       <c r="A531" s="6" t="s">
         <v>1596</v>
       </c>
@@ -22426,7 +23334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="532" spans="1:8" ht="15.75">
+    <row r="532" spans="1:8" ht="15.5">
       <c r="A532" s="6" t="s">
         <v>1599</v>
       </c>
@@ -22452,7 +23360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="533" spans="1:8" ht="15.75">
+    <row r="533" spans="1:8" ht="15.5">
       <c r="A533" s="6" t="s">
         <v>1602</v>
       </c>
@@ -22478,7 +23386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="534" spans="1:8" ht="15.75">
+    <row r="534" spans="1:8" ht="15.5">
       <c r="A534" s="6" t="s">
         <v>1605</v>
       </c>
@@ -22504,7 +23412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="535" spans="1:8" ht="15.75">
+    <row r="535" spans="1:8" ht="15.5">
       <c r="A535" s="6" t="s">
         <v>1608</v>
       </c>
@@ -22530,7 +23438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="536" spans="1:8" ht="15.75">
+    <row r="536" spans="1:8" ht="15.5">
       <c r="A536" s="6" t="s">
         <v>1611</v>
       </c>
@@ -22556,7 +23464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="537" spans="1:8" ht="15.75">
+    <row r="537" spans="1:8" ht="15.5">
       <c r="A537" s="6" t="s">
         <v>1614</v>
       </c>
@@ -22582,7 +23490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="538" spans="1:8" ht="15.75">
+    <row r="538" spans="1:8" ht="15.5">
       <c r="A538" s="6" t="s">
         <v>1617</v>
       </c>
@@ -22608,7 +23516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="539" spans="1:8" ht="15.75">
+    <row r="539" spans="1:8" ht="15.5">
       <c r="A539" s="6" t="s">
         <v>1620</v>
       </c>
@@ -22634,7 +23542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="540" spans="1:8" ht="15.75">
+    <row r="540" spans="1:8" ht="15.5">
       <c r="A540" s="6" t="s">
         <v>1623</v>
       </c>
@@ -22660,7 +23568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="541" spans="1:8" ht="15.75">
+    <row r="541" spans="1:8" ht="15.5">
       <c r="A541" s="6" t="s">
         <v>1626</v>
       </c>
@@ -22686,7 +23594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="542" spans="1:8" ht="15.75">
+    <row r="542" spans="1:8" ht="15.5">
       <c r="A542" s="6" t="s">
         <v>1629</v>
       </c>
@@ -22712,7 +23620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="543" spans="1:8" ht="15.75">
+    <row r="543" spans="1:8" ht="15.5">
       <c r="A543" s="6" t="s">
         <v>1632</v>
       </c>
@@ -22738,7 +23646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="544" spans="1:8" ht="15.75">
+    <row r="544" spans="1:8" ht="15.5">
       <c r="A544" s="6" t="s">
         <v>1635</v>
       </c>
@@ -22764,7 +23672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="545" spans="1:8" ht="15.75">
+    <row r="545" spans="1:8" ht="15.5">
       <c r="A545" s="6" t="s">
         <v>1638</v>
       </c>
@@ -22790,7 +23698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="546" spans="1:8" ht="15.75">
+    <row r="546" spans="1:8" ht="15.5">
       <c r="A546" s="6" t="s">
         <v>1641</v>
       </c>
@@ -22816,7 +23724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="547" spans="1:8" ht="15.75">
+    <row r="547" spans="1:8" ht="15.5">
       <c r="A547" s="6" t="s">
         <v>1644</v>
       </c>
@@ -22842,7 +23750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="548" spans="1:8" ht="15.75">
+    <row r="548" spans="1:8" ht="15.5">
       <c r="A548" s="6" t="s">
         <v>1647</v>
       </c>
@@ -22868,7 +23776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="549" spans="1:8" ht="15.75">
+    <row r="549" spans="1:8" ht="15.5">
       <c r="A549" s="6" t="s">
         <v>1650</v>
       </c>
@@ -22894,7 +23802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="550" spans="1:8" ht="15.75">
+    <row r="550" spans="1:8" ht="15.5">
       <c r="A550" s="6" t="s">
         <v>1653</v>
       </c>
@@ -22920,7 +23828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="551" spans="1:8" ht="15.75">
+    <row r="551" spans="1:8" ht="15.5">
       <c r="A551" s="6" t="s">
         <v>1656</v>
       </c>
@@ -22946,7 +23854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="552" spans="1:8" ht="15.75">
+    <row r="552" spans="1:8" ht="15.5">
       <c r="A552" s="6" t="s">
         <v>1659</v>
       </c>
@@ -22972,7 +23880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="553" spans="1:8" ht="15.75">
+    <row r="553" spans="1:8" ht="15.5">
       <c r="A553" s="6" t="s">
         <v>1662</v>
       </c>
@@ -22998,7 +23906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="554" spans="1:8" ht="15.75">
+    <row r="554" spans="1:8" ht="15.5">
       <c r="A554" s="6" t="s">
         <v>1665</v>
       </c>
@@ -23024,7 +23932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="555" spans="1:8" ht="15.75">
+    <row r="555" spans="1:8" ht="15.5">
       <c r="A555" s="6" t="s">
         <v>1668</v>
       </c>
@@ -23050,7 +23958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="556" spans="1:8" ht="15.75">
+    <row r="556" spans="1:8" ht="15.5">
       <c r="A556" s="6" t="s">
         <v>1671</v>
       </c>
@@ -23076,7 +23984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="557" spans="1:8" ht="15.75">
+    <row r="557" spans="1:8" ht="15.5">
       <c r="A557" s="6" t="s">
         <v>1674</v>
       </c>
@@ -23102,7 +24010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="558" spans="1:8" ht="15.75">
+    <row r="558" spans="1:8" ht="15.5">
       <c r="A558" s="6" t="s">
         <v>1677</v>
       </c>
@@ -23128,7 +24036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="559" spans="1:8" ht="15.75">
+    <row r="559" spans="1:8" ht="15.5">
       <c r="A559" s="6" t="s">
         <v>1680</v>
       </c>
@@ -23154,7 +24062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="560" spans="1:8" ht="15.75">
+    <row r="560" spans="1:8" ht="15.5">
       <c r="A560" s="6" t="s">
         <v>1683</v>
       </c>
@@ -23180,7 +24088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="561" spans="1:8" ht="15.75">
+    <row r="561" spans="1:8" ht="15.5">
       <c r="A561" s="6" t="s">
         <v>1686</v>
       </c>
@@ -23206,7 +24114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="562" spans="1:8" ht="15.75">
+    <row r="562" spans="1:8" ht="15.5">
       <c r="A562" s="6" t="s">
         <v>1689</v>
       </c>
@@ -23232,7 +24140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="563" spans="1:8" ht="15.75">
+    <row r="563" spans="1:8" ht="15.5">
       <c r="A563" s="6" t="s">
         <v>1692</v>
       </c>
@@ -23258,7 +24166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="564" spans="1:8" ht="15.75">
+    <row r="564" spans="1:8" ht="15.5">
       <c r="A564" s="6" t="s">
         <v>1695</v>
       </c>
@@ -23284,7 +24192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="565" spans="1:8" ht="15.75">
+    <row r="565" spans="1:8" ht="15.5">
       <c r="A565" s="6" t="s">
         <v>1698</v>
       </c>
@@ -23310,7 +24218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="566" spans="1:8" ht="15.75">
+    <row r="566" spans="1:8" ht="15.5">
       <c r="A566" s="6" t="s">
         <v>1701</v>
       </c>
@@ -23336,7 +24244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="567" spans="1:8" ht="15.75">
+    <row r="567" spans="1:8" ht="15.5">
       <c r="A567" s="6" t="s">
         <v>1704</v>
       </c>
@@ -23362,7 +24270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="568" spans="1:8" ht="15.75">
+    <row r="568" spans="1:8" ht="15.5">
       <c r="A568" s="6" t="s">
         <v>1707</v>
       </c>
@@ -23388,7 +24296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="569" spans="1:8" ht="15.75">
+    <row r="569" spans="1:8" ht="15.5">
       <c r="A569" s="6" t="s">
         <v>1710</v>
       </c>
@@ -23414,7 +24322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="570" spans="1:8" ht="15.75">
+    <row r="570" spans="1:8" ht="15.5">
       <c r="A570" s="6" t="s">
         <v>1713</v>
       </c>
@@ -23440,7 +24348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="571" spans="1:8" ht="15.75">
+    <row r="571" spans="1:8" ht="15.5">
       <c r="A571" s="6" t="s">
         <v>1715</v>
       </c>
@@ -23466,7 +24374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="572" spans="1:8" ht="15.75">
+    <row r="572" spans="1:8" ht="15.5">
       <c r="A572" s="6" t="s">
         <v>1718</v>
       </c>
@@ -23492,7 +24400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="573" spans="1:8" ht="15.75">
+    <row r="573" spans="1:8" ht="15.5">
       <c r="A573" s="6" t="s">
         <v>1721</v>
       </c>
@@ -23518,7 +24426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="574" spans="1:8" ht="15.75">
+    <row r="574" spans="1:8" ht="15.5">
       <c r="A574" s="6" t="s">
         <v>1724</v>
       </c>
@@ -23544,7 +24452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="575" spans="1:8" ht="15.75">
+    <row r="575" spans="1:8" ht="15.5">
       <c r="A575" s="6" t="s">
         <v>1727</v>
       </c>
@@ -23570,7 +24478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="576" spans="1:8" ht="15.75">
+    <row r="576" spans="1:8" ht="15.5">
       <c r="A576" s="6" t="s">
         <v>1730</v>
       </c>
@@ -23596,7 +24504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="577" spans="1:8" ht="15.75">
+    <row r="577" spans="1:8" ht="15.5">
       <c r="A577" s="6" t="s">
         <v>1733</v>
       </c>
@@ -23622,7 +24530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="578" spans="1:8" ht="15.75">
+    <row r="578" spans="1:8" ht="15.5">
       <c r="A578" s="6" t="s">
         <v>1736</v>
       </c>
@@ -23648,7 +24556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="579" spans="1:8" ht="15.75">
+    <row r="579" spans="1:8" ht="15.5">
       <c r="A579" s="6" t="s">
         <v>1739</v>
       </c>
@@ -23674,7 +24582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="580" spans="1:8" ht="15.75">
+    <row r="580" spans="1:8" ht="15.5">
       <c r="A580" s="6" t="s">
         <v>1742</v>
       </c>
@@ -23700,7 +24608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="581" spans="1:8" ht="15.75">
+    <row r="581" spans="1:8" ht="15.5">
       <c r="A581" s="6" t="s">
         <v>1745</v>
       </c>
@@ -23726,7 +24634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="582" spans="1:8" ht="15.75">
+    <row r="582" spans="1:8" ht="15.5">
       <c r="A582" s="6" t="s">
         <v>1748</v>
       </c>
@@ -23752,7 +24660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="583" spans="1:8" ht="15.75">
+    <row r="583" spans="1:8" ht="15.5">
       <c r="A583" s="6" t="s">
         <v>1751</v>
       </c>
@@ -23778,7 +24686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="584" spans="1:8" ht="15.75">
+    <row r="584" spans="1:8" ht="15.5">
       <c r="A584" s="6" t="s">
         <v>1754</v>
       </c>
@@ -23804,7 +24712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="585" spans="1:8" ht="15.75">
+    <row r="585" spans="1:8" ht="15.5">
       <c r="A585" s="6" t="s">
         <v>1757</v>
       </c>
@@ -23830,7 +24738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="586" spans="1:8" ht="15.75">
+    <row r="586" spans="1:8" ht="15.5">
       <c r="A586" s="6" t="s">
         <v>1760</v>
       </c>
@@ -23856,7 +24764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="587" spans="1:8" ht="15.75">
+    <row r="587" spans="1:8" ht="15.5">
       <c r="A587" s="6" t="s">
         <v>1763</v>
       </c>
@@ -23882,7 +24790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="588" spans="1:8" ht="15.75">
+    <row r="588" spans="1:8" ht="15.5">
       <c r="A588" s="6" t="s">
         <v>1766</v>
       </c>
@@ -23908,7 +24816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="589" spans="1:8" ht="15.75">
+    <row r="589" spans="1:8" ht="15.5">
       <c r="A589" s="6" t="s">
         <v>1769</v>
       </c>
@@ -23934,7 +24842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="590" spans="1:8" ht="15.75">
+    <row r="590" spans="1:8" ht="15.5">
       <c r="A590" s="6" t="s">
         <v>1772</v>
       </c>
@@ -23960,7 +24868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="591" spans="1:8" ht="15.75">
+    <row r="591" spans="1:8" ht="15.5">
       <c r="A591" s="6" t="s">
         <v>1775</v>
       </c>
@@ -23986,7 +24894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="592" spans="1:8" ht="15.75">
+    <row r="592" spans="1:8" ht="15.5">
       <c r="A592" s="6" t="s">
         <v>1778</v>
       </c>
@@ -24012,7 +24920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="593" spans="1:8" ht="15.75">
+    <row r="593" spans="1:8" ht="15.5">
       <c r="A593" s="6" t="s">
         <v>1781</v>
       </c>
@@ -24038,7 +24946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="594" spans="1:8" ht="15.75">
+    <row r="594" spans="1:8" ht="15.5">
       <c r="A594" s="6" t="s">
         <v>1784</v>
       </c>
@@ -24064,7 +24972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="595" spans="1:8" ht="15.75">
+    <row r="595" spans="1:8" ht="15.5">
       <c r="A595" s="6" t="s">
         <v>1787</v>
       </c>
@@ -24090,7 +24998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="596" spans="1:8" ht="15.75">
+    <row r="596" spans="1:8" ht="15.5">
       <c r="A596" s="6" t="s">
         <v>1790</v>
       </c>
@@ -24116,7 +25024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="597" spans="1:8" ht="15.75">
+    <row r="597" spans="1:8" ht="15.5">
       <c r="A597" s="6" t="s">
         <v>1793</v>
       </c>
@@ -24142,7 +25050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="598" spans="1:8" ht="15.75">
+    <row r="598" spans="1:8" ht="15.5">
       <c r="A598" s="6" t="s">
         <v>1796</v>
       </c>
@@ -24168,7 +25076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="599" spans="1:8" ht="15.75">
+    <row r="599" spans="1:8" ht="15.5">
       <c r="A599" s="6" t="s">
         <v>1799</v>
       </c>
@@ -24194,7 +25102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="600" spans="1:8" ht="15.75">
+    <row r="600" spans="1:8" ht="15.5">
       <c r="A600" s="6" t="s">
         <v>1802</v>
       </c>
@@ -24220,7 +25128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="601" spans="1:8" ht="15.75">
+    <row r="601" spans="1:8" ht="15.5">
       <c r="A601" s="6" t="s">
         <v>1805</v>
       </c>
@@ -24246,7 +25154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="602" spans="1:8" ht="15.75">
+    <row r="602" spans="1:8" ht="15.5">
       <c r="A602" s="6" t="s">
         <v>1808</v>
       </c>
@@ -24272,7 +25180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="603" spans="1:8" ht="15.75">
+    <row r="603" spans="1:8" ht="15.5">
       <c r="A603" s="6" t="s">
         <v>1811</v>
       </c>
@@ -24298,7 +25206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="604" spans="1:8" ht="15.75">
+    <row r="604" spans="1:8" ht="15.5">
       <c r="A604" s="6" t="s">
         <v>1814</v>
       </c>
@@ -24324,7 +25232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="605" spans="1:8" ht="15.75">
+    <row r="605" spans="1:8" ht="15.5">
       <c r="A605" s="6" t="s">
         <v>1817</v>
       </c>
@@ -24350,7 +25258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="606" spans="1:8" ht="15.75">
+    <row r="606" spans="1:8" ht="15.5">
       <c r="A606" s="6" t="s">
         <v>1820</v>
       </c>
@@ -24376,7 +25284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="607" spans="1:8" ht="15.75">
+    <row r="607" spans="1:8" ht="15.5">
       <c r="A607" s="6" t="s">
         <v>1823</v>
       </c>
@@ -24402,7 +25310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="608" spans="1:8" ht="15.75">
+    <row r="608" spans="1:8" ht="15.5">
       <c r="A608" s="6" t="s">
         <v>1826</v>
       </c>
@@ -24428,7 +25336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="609" spans="1:8" ht="15.75">
+    <row r="609" spans="1:8" ht="15.5">
       <c r="A609" s="6" t="s">
         <v>1829</v>
       </c>
@@ -24454,7 +25362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="610" spans="1:8" ht="15.75">
+    <row r="610" spans="1:8" ht="15.5">
       <c r="A610" s="6" t="s">
         <v>1832</v>
       </c>
@@ -24480,7 +25388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="611" spans="1:8" ht="15.75">
+    <row r="611" spans="1:8" ht="15.5">
       <c r="A611" s="6" t="s">
         <v>1835</v>
       </c>
@@ -24506,7 +25414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="612" spans="1:8" ht="15.75">
+    <row r="612" spans="1:8" ht="15.5">
       <c r="A612" s="6" t="s">
         <v>1838</v>
       </c>
@@ -24532,7 +25440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="613" spans="1:8" ht="15.75">
+    <row r="613" spans="1:8" ht="15.5">
       <c r="A613" s="6" t="s">
         <v>1841</v>
       </c>
@@ -24558,7 +25466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="614" spans="1:8" ht="15.75">
+    <row r="614" spans="1:8" ht="15.5">
       <c r="A614" s="6" t="s">
         <v>1844</v>
       </c>
@@ -24584,7 +25492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="615" spans="1:8" ht="15.75">
+    <row r="615" spans="1:8" ht="15.5">
       <c r="A615" s="6" t="s">
         <v>1847</v>
       </c>
@@ -24610,7 +25518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="616" spans="1:8" ht="15.75">
+    <row r="616" spans="1:8" ht="15.5">
       <c r="A616" s="6" t="s">
         <v>1850</v>
       </c>
@@ -24636,7 +25544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="617" spans="1:8" ht="15.75">
+    <row r="617" spans="1:8" ht="15.5">
       <c r="A617" s="6" t="s">
         <v>1853</v>
       </c>
@@ -24662,7 +25570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="618" spans="1:8" ht="15.75">
+    <row r="618" spans="1:8" ht="15.5">
       <c r="A618" s="6" t="s">
         <v>1856</v>
       </c>
@@ -24688,7 +25596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="619" spans="1:8" ht="15.75">
+    <row r="619" spans="1:8" ht="15.5">
       <c r="A619" s="6" t="s">
         <v>1859</v>
       </c>
@@ -32355,6 +33263,2606 @@
         <v>12</v>
       </c>
       <c r="H913" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="914" spans="1:8">
+      <c r="A914" t="s">
+        <v>2743</v>
+      </c>
+      <c r="B914" t="s">
+        <v>9</v>
+      </c>
+      <c r="C914" t="s">
+        <v>2744</v>
+      </c>
+      <c r="D914" t="s">
+        <v>2745</v>
+      </c>
+      <c r="E914" t="s">
+        <v>12</v>
+      </c>
+      <c r="F914" t="s">
+        <v>12</v>
+      </c>
+      <c r="G914" t="s">
+        <v>12</v>
+      </c>
+      <c r="H914" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="915" spans="1:8">
+      <c r="A915" t="s">
+        <v>2746</v>
+      </c>
+      <c r="B915" t="s">
+        <v>14</v>
+      </c>
+      <c r="C915" t="s">
+        <v>2747</v>
+      </c>
+      <c r="D915" t="s">
+        <v>2748</v>
+      </c>
+      <c r="E915" t="s">
+        <v>12</v>
+      </c>
+      <c r="F915" t="s">
+        <v>12</v>
+      </c>
+      <c r="G915" t="s">
+        <v>12</v>
+      </c>
+      <c r="H915" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="916" spans="1:8">
+      <c r="A916" t="s">
+        <v>2749</v>
+      </c>
+      <c r="B916" t="s">
+        <v>14</v>
+      </c>
+      <c r="C916" t="s">
+        <v>2750</v>
+      </c>
+      <c r="D916" t="s">
+        <v>2751</v>
+      </c>
+      <c r="E916" t="s">
+        <v>23</v>
+      </c>
+      <c r="F916" t="s">
+        <v>23</v>
+      </c>
+      <c r="G916" t="s">
+        <v>23</v>
+      </c>
+      <c r="H916" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="917" spans="1:8">
+      <c r="A917" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B917" t="s">
+        <v>9</v>
+      </c>
+      <c r="C917" t="s">
+        <v>2753</v>
+      </c>
+      <c r="D917" t="s">
+        <v>2754</v>
+      </c>
+      <c r="E917" t="s">
+        <v>23</v>
+      </c>
+      <c r="F917" t="s">
+        <v>23</v>
+      </c>
+      <c r="G917" t="s">
+        <v>23</v>
+      </c>
+      <c r="H917" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="918" spans="1:8">
+      <c r="A918" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B918" t="s">
+        <v>9</v>
+      </c>
+      <c r="C918" t="s">
+        <v>2756</v>
+      </c>
+      <c r="D918" t="s">
+        <v>2757</v>
+      </c>
+      <c r="E918" t="s">
+        <v>12</v>
+      </c>
+      <c r="F918" t="s">
+        <v>12</v>
+      </c>
+      <c r="G918" t="s">
+        <v>12</v>
+      </c>
+      <c r="H918" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="919" spans="1:8">
+      <c r="A919" t="s">
+        <v>2758</v>
+      </c>
+      <c r="B919" t="s">
+        <v>9</v>
+      </c>
+      <c r="C919" t="s">
+        <v>2759</v>
+      </c>
+      <c r="D919" t="s">
+        <v>2760</v>
+      </c>
+      <c r="E919" t="s">
+        <v>12</v>
+      </c>
+      <c r="F919" t="s">
+        <v>12</v>
+      </c>
+      <c r="G919" t="s">
+        <v>12</v>
+      </c>
+      <c r="H919" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="920" spans="1:8">
+      <c r="A920" t="s">
+        <v>2761</v>
+      </c>
+      <c r="B920" t="s">
+        <v>9</v>
+      </c>
+      <c r="C920" t="s">
+        <v>2762</v>
+      </c>
+      <c r="D920" t="s">
+        <v>2763</v>
+      </c>
+      <c r="E920" t="s">
+        <v>12</v>
+      </c>
+      <c r="F920" t="s">
+        <v>12</v>
+      </c>
+      <c r="G920" t="s">
+        <v>12</v>
+      </c>
+      <c r="H920" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="921" spans="1:8">
+      <c r="A921" t="s">
+        <v>2764</v>
+      </c>
+      <c r="B921" t="s">
+        <v>9</v>
+      </c>
+      <c r="C921" t="s">
+        <v>2765</v>
+      </c>
+      <c r="D921" t="s">
+        <v>2766</v>
+      </c>
+      <c r="E921" t="s">
+        <v>12</v>
+      </c>
+      <c r="F921" t="s">
+        <v>23</v>
+      </c>
+      <c r="G921" t="s">
+        <v>12</v>
+      </c>
+      <c r="H921" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="922" spans="1:8">
+      <c r="A922" t="s">
+        <v>2767</v>
+      </c>
+      <c r="B922" t="s">
+        <v>14</v>
+      </c>
+      <c r="C922" t="s">
+        <v>2768</v>
+      </c>
+      <c r="D922" t="s">
+        <v>2769</v>
+      </c>
+      <c r="E922" t="s">
+        <v>12</v>
+      </c>
+      <c r="F922" t="s">
+        <v>12</v>
+      </c>
+      <c r="G922" t="s">
+        <v>12</v>
+      </c>
+      <c r="H922" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="923" spans="1:8">
+      <c r="A923" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B923" t="s">
+        <v>9</v>
+      </c>
+      <c r="C923" t="s">
+        <v>2771</v>
+      </c>
+      <c r="D923" t="s">
+        <v>2772</v>
+      </c>
+      <c r="E923" t="s">
+        <v>23</v>
+      </c>
+      <c r="F923" t="s">
+        <v>23</v>
+      </c>
+      <c r="G923" t="s">
+        <v>23</v>
+      </c>
+      <c r="H923" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="924" spans="1:8">
+      <c r="A924" t="s">
+        <v>2773</v>
+      </c>
+      <c r="B924" t="s">
+        <v>9</v>
+      </c>
+      <c r="C924" t="s">
+        <v>2774</v>
+      </c>
+      <c r="D924" t="s">
+        <v>2775</v>
+      </c>
+      <c r="E924" t="s">
+        <v>12</v>
+      </c>
+      <c r="F924" t="s">
+        <v>23</v>
+      </c>
+      <c r="G924" t="s">
+        <v>12</v>
+      </c>
+      <c r="H924" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="925" spans="1:8">
+      <c r="A925" t="s">
+        <v>2776</v>
+      </c>
+      <c r="B925" t="s">
+        <v>9</v>
+      </c>
+      <c r="C925" t="s">
+        <v>2777</v>
+      </c>
+      <c r="D925" t="s">
+        <v>2778</v>
+      </c>
+      <c r="E925" t="s">
+        <v>12</v>
+      </c>
+      <c r="F925" t="s">
+        <v>12</v>
+      </c>
+      <c r="G925" t="s">
+        <v>12</v>
+      </c>
+      <c r="H925" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="926" spans="1:8">
+      <c r="A926" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B926" t="s">
+        <v>14</v>
+      </c>
+      <c r="C926" t="s">
+        <v>2780</v>
+      </c>
+      <c r="D926" t="s">
+        <v>2781</v>
+      </c>
+      <c r="E926" t="s">
+        <v>12</v>
+      </c>
+      <c r="F926" t="s">
+        <v>23</v>
+      </c>
+      <c r="G926" t="s">
+        <v>12</v>
+      </c>
+      <c r="H926" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="927" spans="1:8">
+      <c r="A927" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B927" t="s">
+        <v>14</v>
+      </c>
+      <c r="C927" t="s">
+        <v>2783</v>
+      </c>
+      <c r="D927" t="s">
+        <v>2784</v>
+      </c>
+      <c r="E927" t="s">
+        <v>12</v>
+      </c>
+      <c r="F927" t="s">
+        <v>12</v>
+      </c>
+      <c r="G927" t="s">
+        <v>12</v>
+      </c>
+      <c r="H927" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="928" spans="1:8">
+      <c r="A928" t="s">
+        <v>2785</v>
+      </c>
+      <c r="B928" t="s">
+        <v>14</v>
+      </c>
+      <c r="C928" t="s">
+        <v>2786</v>
+      </c>
+      <c r="D928" t="s">
+        <v>2787</v>
+      </c>
+      <c r="E928" t="s">
+        <v>12</v>
+      </c>
+      <c r="F928" t="s">
+        <v>12</v>
+      </c>
+      <c r="G928" t="s">
+        <v>12</v>
+      </c>
+      <c r="H928" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="929" spans="1:8">
+      <c r="A929" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B929" t="s">
+        <v>14</v>
+      </c>
+      <c r="C929" t="s">
+        <v>2789</v>
+      </c>
+      <c r="D929" t="s">
+        <v>2790</v>
+      </c>
+      <c r="E929" t="s">
+        <v>12</v>
+      </c>
+      <c r="F929" t="s">
+        <v>12</v>
+      </c>
+      <c r="G929" t="s">
+        <v>12</v>
+      </c>
+      <c r="H929" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="930" spans="1:8">
+      <c r="A930" t="s">
+        <v>2791</v>
+      </c>
+      <c r="B930" t="s">
+        <v>14</v>
+      </c>
+      <c r="C930" t="s">
+        <v>2792</v>
+      </c>
+      <c r="D930" t="s">
+        <v>2793</v>
+      </c>
+      <c r="E930" t="s">
+        <v>12</v>
+      </c>
+      <c r="F930" t="s">
+        <v>12</v>
+      </c>
+      <c r="G930" t="s">
+        <v>12</v>
+      </c>
+      <c r="H930" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="931" spans="1:8">
+      <c r="A931" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B931" t="s">
+        <v>14</v>
+      </c>
+      <c r="C931" t="s">
+        <v>2795</v>
+      </c>
+      <c r="D931" t="s">
+        <v>2796</v>
+      </c>
+      <c r="E931" t="s">
+        <v>12</v>
+      </c>
+      <c r="F931" t="s">
+        <v>12</v>
+      </c>
+      <c r="G931" t="s">
+        <v>12</v>
+      </c>
+      <c r="H931" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="932" spans="1:8">
+      <c r="A932" t="s">
+        <v>2797</v>
+      </c>
+      <c r="B932" t="s">
+        <v>14</v>
+      </c>
+      <c r="C932" t="s">
+        <v>2798</v>
+      </c>
+      <c r="D932" t="s">
+        <v>2799</v>
+      </c>
+      <c r="E932" t="s">
+        <v>12</v>
+      </c>
+      <c r="F932" t="s">
+        <v>12</v>
+      </c>
+      <c r="G932" t="s">
+        <v>12</v>
+      </c>
+      <c r="H932" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="933" spans="1:8">
+      <c r="A933" t="s">
+        <v>2800</v>
+      </c>
+      <c r="B933" t="s">
+        <v>14</v>
+      </c>
+      <c r="C933" t="s">
+        <v>2801</v>
+      </c>
+      <c r="D933" t="s">
+        <v>2802</v>
+      </c>
+      <c r="E933" t="s">
+        <v>12</v>
+      </c>
+      <c r="F933" t="s">
+        <v>12</v>
+      </c>
+      <c r="G933" t="s">
+        <v>12</v>
+      </c>
+      <c r="H933" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="934" spans="1:8">
+      <c r="A934" t="s">
+        <v>2803</v>
+      </c>
+      <c r="B934" t="s">
+        <v>14</v>
+      </c>
+      <c r="C934" t="s">
+        <v>2804</v>
+      </c>
+      <c r="D934" t="s">
+        <v>2805</v>
+      </c>
+      <c r="E934" t="s">
+        <v>12</v>
+      </c>
+      <c r="F934" t="s">
+        <v>12</v>
+      </c>
+      <c r="G934" t="s">
+        <v>12</v>
+      </c>
+      <c r="H934" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="935" spans="1:8">
+      <c r="A935" t="s">
+        <v>2806</v>
+      </c>
+      <c r="B935" t="s">
+        <v>14</v>
+      </c>
+      <c r="C935" t="s">
+        <v>2807</v>
+      </c>
+      <c r="D935" t="s">
+        <v>2808</v>
+      </c>
+      <c r="E935" t="s">
+        <v>12</v>
+      </c>
+      <c r="F935" t="s">
+        <v>12</v>
+      </c>
+      <c r="G935" t="s">
+        <v>12</v>
+      </c>
+      <c r="H935" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="936" spans="1:8">
+      <c r="A936" t="s">
+        <v>2809</v>
+      </c>
+      <c r="B936" t="s">
+        <v>9</v>
+      </c>
+      <c r="C936" t="s">
+        <v>2810</v>
+      </c>
+      <c r="D936" t="s">
+        <v>2811</v>
+      </c>
+      <c r="E936" t="s">
+        <v>12</v>
+      </c>
+      <c r="F936" t="s">
+        <v>12</v>
+      </c>
+      <c r="G936" t="s">
+        <v>12</v>
+      </c>
+      <c r="H936" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="937" spans="1:8">
+      <c r="A937" t="s">
+        <v>2812</v>
+      </c>
+      <c r="B937" t="s">
+        <v>9</v>
+      </c>
+      <c r="C937" t="s">
+        <v>2813</v>
+      </c>
+      <c r="D937" t="s">
+        <v>2814</v>
+      </c>
+      <c r="E937" t="s">
+        <v>12</v>
+      </c>
+      <c r="F937" t="s">
+        <v>23</v>
+      </c>
+      <c r="G937" t="s">
+        <v>12</v>
+      </c>
+      <c r="H937" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="938" spans="1:8">
+      <c r="A938" t="s">
+        <v>2815</v>
+      </c>
+      <c r="B938" t="s">
+        <v>14</v>
+      </c>
+      <c r="C938" t="s">
+        <v>2816</v>
+      </c>
+      <c r="D938" t="s">
+        <v>2817</v>
+      </c>
+      <c r="E938" t="s">
+        <v>12</v>
+      </c>
+      <c r="F938" t="s">
+        <v>12</v>
+      </c>
+      <c r="G938" t="s">
+        <v>12</v>
+      </c>
+      <c r="H938" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="939" spans="1:8">
+      <c r="A939" t="s">
+        <v>2818</v>
+      </c>
+      <c r="B939" t="s">
+        <v>14</v>
+      </c>
+      <c r="C939" t="s">
+        <v>2819</v>
+      </c>
+      <c r="D939" t="s">
+        <v>2820</v>
+      </c>
+      <c r="E939" t="s">
+        <v>12</v>
+      </c>
+      <c r="F939" t="s">
+        <v>12</v>
+      </c>
+      <c r="G939" t="s">
+        <v>12</v>
+      </c>
+      <c r="H939" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="940" spans="1:8">
+      <c r="A940" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B940" t="s">
+        <v>14</v>
+      </c>
+      <c r="C940" t="s">
+        <v>2822</v>
+      </c>
+      <c r="D940" t="s">
+        <v>2823</v>
+      </c>
+      <c r="E940" t="s">
+        <v>12</v>
+      </c>
+      <c r="F940" t="s">
+        <v>12</v>
+      </c>
+      <c r="G940" t="s">
+        <v>12</v>
+      </c>
+      <c r="H940" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="941" spans="1:8">
+      <c r="A941" t="s">
+        <v>2824</v>
+      </c>
+      <c r="B941" t="s">
+        <v>9</v>
+      </c>
+      <c r="C941" t="s">
+        <v>2825</v>
+      </c>
+      <c r="D941" t="s">
+        <v>2826</v>
+      </c>
+      <c r="E941" t="s">
+        <v>12</v>
+      </c>
+      <c r="F941" t="s">
+        <v>12</v>
+      </c>
+      <c r="G941" t="s">
+        <v>12</v>
+      </c>
+      <c r="H941" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="942" spans="1:8">
+      <c r="A942" t="s">
+        <v>2827</v>
+      </c>
+      <c r="B942" t="s">
+        <v>14</v>
+      </c>
+      <c r="C942" t="s">
+        <v>2828</v>
+      </c>
+      <c r="D942" t="s">
+        <v>2829</v>
+      </c>
+      <c r="E942" t="s">
+        <v>12</v>
+      </c>
+      <c r="F942" t="s">
+        <v>12</v>
+      </c>
+      <c r="G942" t="s">
+        <v>12</v>
+      </c>
+      <c r="H942" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="943" spans="1:8">
+      <c r="A943" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B943" t="s">
+        <v>14</v>
+      </c>
+      <c r="C943" t="s">
+        <v>2831</v>
+      </c>
+      <c r="D943" t="s">
+        <v>2832</v>
+      </c>
+      <c r="E943" t="s">
+        <v>12</v>
+      </c>
+      <c r="F943" t="s">
+        <v>12</v>
+      </c>
+      <c r="G943" t="s">
+        <v>12</v>
+      </c>
+      <c r="H943" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="944" spans="1:8">
+      <c r="A944" t="s">
+        <v>2833</v>
+      </c>
+      <c r="B944" t="s">
+        <v>9</v>
+      </c>
+      <c r="C944" t="s">
+        <v>2834</v>
+      </c>
+      <c r="D944" t="s">
+        <v>2835</v>
+      </c>
+      <c r="E944" t="s">
+        <v>23</v>
+      </c>
+      <c r="F944" t="s">
+        <v>23</v>
+      </c>
+      <c r="G944" t="s">
+        <v>23</v>
+      </c>
+      <c r="H944" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="945" spans="1:8">
+      <c r="A945" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B945" t="s">
+        <v>9</v>
+      </c>
+      <c r="C945" t="s">
+        <v>2837</v>
+      </c>
+      <c r="D945" t="s">
+        <v>2838</v>
+      </c>
+      <c r="E945" t="s">
+        <v>12</v>
+      </c>
+      <c r="F945" t="s">
+        <v>12</v>
+      </c>
+      <c r="G945" t="s">
+        <v>12</v>
+      </c>
+      <c r="H945" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="946" spans="1:8">
+      <c r="A946" t="s">
+        <v>2839</v>
+      </c>
+      <c r="B946" t="s">
+        <v>14</v>
+      </c>
+      <c r="C946" t="s">
+        <v>2840</v>
+      </c>
+      <c r="D946" t="s">
+        <v>2841</v>
+      </c>
+      <c r="E946" t="s">
+        <v>12</v>
+      </c>
+      <c r="F946" t="s">
+        <v>23</v>
+      </c>
+      <c r="G946" t="s">
+        <v>12</v>
+      </c>
+      <c r="H946" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="947" spans="1:8">
+      <c r="A947" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B947" t="s">
+        <v>14</v>
+      </c>
+      <c r="C947" t="s">
+        <v>2843</v>
+      </c>
+      <c r="D947" t="s">
+        <v>2844</v>
+      </c>
+      <c r="E947" t="s">
+        <v>23</v>
+      </c>
+      <c r="F947" t="s">
+        <v>23</v>
+      </c>
+      <c r="G947" t="s">
+        <v>23</v>
+      </c>
+      <c r="H947" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="948" spans="1:8">
+      <c r="A948" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B948" t="s">
+        <v>14</v>
+      </c>
+      <c r="C948" t="s">
+        <v>2846</v>
+      </c>
+      <c r="D948" t="s">
+        <v>2847</v>
+      </c>
+      <c r="E948" t="s">
+        <v>12</v>
+      </c>
+      <c r="F948" t="s">
+        <v>12</v>
+      </c>
+      <c r="G948" t="s">
+        <v>12</v>
+      </c>
+      <c r="H948" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="949" spans="1:8">
+      <c r="A949" t="s">
+        <v>2848</v>
+      </c>
+      <c r="B949" t="s">
+        <v>9</v>
+      </c>
+      <c r="C949" t="s">
+        <v>2849</v>
+      </c>
+      <c r="D949" t="s">
+        <v>2850</v>
+      </c>
+      <c r="E949" t="s">
+        <v>12</v>
+      </c>
+      <c r="F949" t="s">
+        <v>23</v>
+      </c>
+      <c r="G949" t="s">
+        <v>12</v>
+      </c>
+      <c r="H949" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="950" spans="1:8">
+      <c r="A950" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B950" t="s">
+        <v>14</v>
+      </c>
+      <c r="C950" t="s">
+        <v>2852</v>
+      </c>
+      <c r="D950" t="s">
+        <v>2853</v>
+      </c>
+      <c r="E950" t="s">
+        <v>12</v>
+      </c>
+      <c r="F950" t="s">
+        <v>12</v>
+      </c>
+      <c r="G950" t="s">
+        <v>12</v>
+      </c>
+      <c r="H950" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="951" spans="1:8">
+      <c r="A951" t="s">
+        <v>2854</v>
+      </c>
+      <c r="B951" t="s">
+        <v>14</v>
+      </c>
+      <c r="C951" t="s">
+        <v>2855</v>
+      </c>
+      <c r="D951" t="s">
+        <v>2856</v>
+      </c>
+      <c r="E951" t="s">
+        <v>12</v>
+      </c>
+      <c r="F951" t="s">
+        <v>12</v>
+      </c>
+      <c r="G951" t="s">
+        <v>12</v>
+      </c>
+      <c r="H951" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="952" spans="1:8">
+      <c r="A952" t="s">
+        <v>2857</v>
+      </c>
+      <c r="B952" t="s">
+        <v>14</v>
+      </c>
+      <c r="C952" t="s">
+        <v>2858</v>
+      </c>
+      <c r="D952" t="s">
+        <v>2859</v>
+      </c>
+      <c r="E952" t="s">
+        <v>12</v>
+      </c>
+      <c r="F952" t="s">
+        <v>23</v>
+      </c>
+      <c r="G952" t="s">
+        <v>12</v>
+      </c>
+      <c r="H952" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="953" spans="1:8">
+      <c r="A953" t="s">
+        <v>2860</v>
+      </c>
+      <c r="B953" t="s">
+        <v>9</v>
+      </c>
+      <c r="C953" t="s">
+        <v>2861</v>
+      </c>
+      <c r="D953" t="s">
+        <v>2862</v>
+      </c>
+      <c r="E953" t="s">
+        <v>12</v>
+      </c>
+      <c r="F953" t="s">
+        <v>23</v>
+      </c>
+      <c r="G953" t="s">
+        <v>12</v>
+      </c>
+      <c r="H953" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="954" spans="1:8">
+      <c r="A954" t="s">
+        <v>2863</v>
+      </c>
+      <c r="B954" t="s">
+        <v>9</v>
+      </c>
+      <c r="C954" t="s">
+        <v>2864</v>
+      </c>
+      <c r="D954" t="s">
+        <v>2865</v>
+      </c>
+      <c r="E954" t="s">
+        <v>12</v>
+      </c>
+      <c r="F954" t="s">
+        <v>12</v>
+      </c>
+      <c r="G954" t="s">
+        <v>12</v>
+      </c>
+      <c r="H954" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="955" spans="1:8">
+      <c r="A955" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B955" t="s">
+        <v>9</v>
+      </c>
+      <c r="C955" t="s">
+        <v>2867</v>
+      </c>
+      <c r="D955" t="s">
+        <v>2868</v>
+      </c>
+      <c r="E955" t="s">
+        <v>12</v>
+      </c>
+      <c r="F955" t="s">
+        <v>23</v>
+      </c>
+      <c r="G955" t="s">
+        <v>12</v>
+      </c>
+      <c r="H955" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="956" spans="1:8">
+      <c r="A956" t="s">
+        <v>2869</v>
+      </c>
+      <c r="B956" t="s">
+        <v>9</v>
+      </c>
+      <c r="C956" t="s">
+        <v>2870</v>
+      </c>
+      <c r="D956" t="s">
+        <v>2871</v>
+      </c>
+      <c r="E956" t="s">
+        <v>12</v>
+      </c>
+      <c r="F956" t="s">
+        <v>12</v>
+      </c>
+      <c r="G956" t="s">
+        <v>12</v>
+      </c>
+      <c r="H956" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="957" spans="1:8">
+      <c r="A957" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B957" t="s">
+        <v>9</v>
+      </c>
+      <c r="C957" t="s">
+        <v>2873</v>
+      </c>
+      <c r="D957" t="s">
+        <v>2874</v>
+      </c>
+      <c r="E957" t="s">
+        <v>12</v>
+      </c>
+      <c r="F957" t="s">
+        <v>12</v>
+      </c>
+      <c r="G957" t="s">
+        <v>12</v>
+      </c>
+      <c r="H957" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="958" spans="1:8">
+      <c r="A958" t="s">
+        <v>2875</v>
+      </c>
+      <c r="B958" t="s">
+        <v>14</v>
+      </c>
+      <c r="C958" t="s">
+        <v>2876</v>
+      </c>
+      <c r="D958" t="s">
+        <v>2877</v>
+      </c>
+      <c r="E958" t="s">
+        <v>12</v>
+      </c>
+      <c r="F958" t="s">
+        <v>12</v>
+      </c>
+      <c r="G958" t="s">
+        <v>12</v>
+      </c>
+      <c r="H958" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="959" spans="1:8">
+      <c r="A959" t="s">
+        <v>2878</v>
+      </c>
+      <c r="B959" t="s">
+        <v>14</v>
+      </c>
+      <c r="C959" t="s">
+        <v>2879</v>
+      </c>
+      <c r="D959" t="s">
+        <v>2880</v>
+      </c>
+      <c r="E959" t="s">
+        <v>12</v>
+      </c>
+      <c r="F959" t="s">
+        <v>12</v>
+      </c>
+      <c r="G959" t="s">
+        <v>12</v>
+      </c>
+      <c r="H959" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="960" spans="1:8">
+      <c r="A960" t="s">
+        <v>2881</v>
+      </c>
+      <c r="B960" t="s">
+        <v>14</v>
+      </c>
+      <c r="C960" t="s">
+        <v>2882</v>
+      </c>
+      <c r="D960" t="s">
+        <v>2883</v>
+      </c>
+      <c r="E960" t="s">
+        <v>12</v>
+      </c>
+      <c r="F960" t="s">
+        <v>23</v>
+      </c>
+      <c r="G960" t="s">
+        <v>12</v>
+      </c>
+      <c r="H960" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="961" spans="1:8">
+      <c r="A961" t="s">
+        <v>2884</v>
+      </c>
+      <c r="B961" t="s">
+        <v>9</v>
+      </c>
+      <c r="C961" t="s">
+        <v>2885</v>
+      </c>
+      <c r="D961" t="s">
+        <v>2886</v>
+      </c>
+      <c r="E961" t="s">
+        <v>12</v>
+      </c>
+      <c r="F961" t="s">
+        <v>12</v>
+      </c>
+      <c r="G961" t="s">
+        <v>12</v>
+      </c>
+      <c r="H961" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="962" spans="1:8">
+      <c r="A962" t="s">
+        <v>2887</v>
+      </c>
+      <c r="B962" t="s">
+        <v>9</v>
+      </c>
+      <c r="C962" t="s">
+        <v>2888</v>
+      </c>
+      <c r="D962" t="s">
+        <v>2889</v>
+      </c>
+      <c r="E962" t="s">
+        <v>12</v>
+      </c>
+      <c r="F962" t="s">
+        <v>12</v>
+      </c>
+      <c r="G962" t="s">
+        <v>12</v>
+      </c>
+      <c r="H962" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="963" spans="1:8">
+      <c r="A963" t="s">
+        <v>2890</v>
+      </c>
+      <c r="B963" t="s">
+        <v>14</v>
+      </c>
+      <c r="C963" t="s">
+        <v>2891</v>
+      </c>
+      <c r="D963" t="s">
+        <v>2892</v>
+      </c>
+      <c r="E963" t="s">
+        <v>12</v>
+      </c>
+      <c r="F963" t="s">
+        <v>12</v>
+      </c>
+      <c r="G963" t="s">
+        <v>12</v>
+      </c>
+      <c r="H963" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="964" spans="1:8">
+      <c r="A964" t="s">
+        <v>2893</v>
+      </c>
+      <c r="B964" t="s">
+        <v>14</v>
+      </c>
+      <c r="C964" t="s">
+        <v>2894</v>
+      </c>
+      <c r="D964" t="s">
+        <v>2895</v>
+      </c>
+      <c r="E964" t="s">
+        <v>12</v>
+      </c>
+      <c r="F964" t="s">
+        <v>23</v>
+      </c>
+      <c r="G964" t="s">
+        <v>12</v>
+      </c>
+      <c r="H964" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="965" spans="1:8">
+      <c r="A965" t="s">
+        <v>2896</v>
+      </c>
+      <c r="B965" t="s">
+        <v>9</v>
+      </c>
+      <c r="C965" t="s">
+        <v>2897</v>
+      </c>
+      <c r="D965" t="s">
+        <v>2898</v>
+      </c>
+      <c r="E965" t="s">
+        <v>12</v>
+      </c>
+      <c r="F965" t="s">
+        <v>12</v>
+      </c>
+      <c r="G965" t="s">
+        <v>12</v>
+      </c>
+      <c r="H965" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="966" spans="1:8">
+      <c r="A966" t="s">
+        <v>2899</v>
+      </c>
+      <c r="B966" t="s">
+        <v>9</v>
+      </c>
+      <c r="C966" t="s">
+        <v>2900</v>
+      </c>
+      <c r="D966" t="s">
+        <v>2901</v>
+      </c>
+      <c r="E966" t="s">
+        <v>12</v>
+      </c>
+      <c r="F966" t="s">
+        <v>12</v>
+      </c>
+      <c r="G966" t="s">
+        <v>12</v>
+      </c>
+      <c r="H966" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="967" spans="1:8">
+      <c r="A967" t="s">
+        <v>2902</v>
+      </c>
+      <c r="B967" t="s">
+        <v>9</v>
+      </c>
+      <c r="C967" t="s">
+        <v>2903</v>
+      </c>
+      <c r="D967" t="s">
+        <v>2904</v>
+      </c>
+      <c r="E967" t="s">
+        <v>12</v>
+      </c>
+      <c r="F967" t="s">
+        <v>23</v>
+      </c>
+      <c r="G967" t="s">
+        <v>12</v>
+      </c>
+      <c r="H967" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="968" spans="1:8">
+      <c r="A968" t="s">
+        <v>2905</v>
+      </c>
+      <c r="B968" t="s">
+        <v>9</v>
+      </c>
+      <c r="C968" t="s">
+        <v>2906</v>
+      </c>
+      <c r="D968" t="s">
+        <v>2907</v>
+      </c>
+      <c r="E968" t="s">
+        <v>12</v>
+      </c>
+      <c r="F968" t="s">
+        <v>12</v>
+      </c>
+      <c r="G968" t="s">
+        <v>12</v>
+      </c>
+      <c r="H968" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="969" spans="1:8">
+      <c r="A969" t="s">
+        <v>2908</v>
+      </c>
+      <c r="B969" t="s">
+        <v>9</v>
+      </c>
+      <c r="C969" t="s">
+        <v>2909</v>
+      </c>
+      <c r="D969" t="s">
+        <v>2910</v>
+      </c>
+      <c r="E969" t="s">
+        <v>23</v>
+      </c>
+      <c r="F969" t="s">
+        <v>23</v>
+      </c>
+      <c r="G969" t="s">
+        <v>23</v>
+      </c>
+      <c r="H969" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="970" spans="1:8">
+      <c r="A970" t="s">
+        <v>2911</v>
+      </c>
+      <c r="B970" t="s">
+        <v>9</v>
+      </c>
+      <c r="C970" t="s">
+        <v>2912</v>
+      </c>
+      <c r="D970" t="s">
+        <v>2913</v>
+      </c>
+      <c r="E970" t="s">
+        <v>12</v>
+      </c>
+      <c r="F970" t="s">
+        <v>12</v>
+      </c>
+      <c r="G970" t="s">
+        <v>12</v>
+      </c>
+      <c r="H970" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="971" spans="1:8">
+      <c r="A971" t="s">
+        <v>2914</v>
+      </c>
+      <c r="B971" t="s">
+        <v>9</v>
+      </c>
+      <c r="C971" t="s">
+        <v>2915</v>
+      </c>
+      <c r="D971" t="s">
+        <v>2916</v>
+      </c>
+      <c r="E971" t="s">
+        <v>12</v>
+      </c>
+      <c r="F971" t="s">
+        <v>12</v>
+      </c>
+      <c r="G971" t="s">
+        <v>12</v>
+      </c>
+      <c r="H971" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="972" spans="1:8">
+      <c r="A972" t="s">
+        <v>2917</v>
+      </c>
+      <c r="B972" t="s">
+        <v>9</v>
+      </c>
+      <c r="C972" t="s">
+        <v>2918</v>
+      </c>
+      <c r="D972" t="s">
+        <v>2919</v>
+      </c>
+      <c r="E972" t="s">
+        <v>23</v>
+      </c>
+      <c r="F972" t="s">
+        <v>23</v>
+      </c>
+      <c r="G972" t="s">
+        <v>23</v>
+      </c>
+      <c r="H972" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="973" spans="1:8">
+      <c r="A973" t="s">
+        <v>2920</v>
+      </c>
+      <c r="B973" t="s">
+        <v>9</v>
+      </c>
+      <c r="C973" t="s">
+        <v>2921</v>
+      </c>
+      <c r="D973" t="s">
+        <v>2922</v>
+      </c>
+      <c r="E973" t="s">
+        <v>12</v>
+      </c>
+      <c r="F973" t="s">
+        <v>23</v>
+      </c>
+      <c r="G973" t="s">
+        <v>12</v>
+      </c>
+      <c r="H973" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="974" spans="1:8">
+      <c r="A974" t="s">
+        <v>2923</v>
+      </c>
+      <c r="B974" t="s">
+        <v>14</v>
+      </c>
+      <c r="C974" t="s">
+        <v>2924</v>
+      </c>
+      <c r="D974" t="s">
+        <v>2925</v>
+      </c>
+      <c r="E974" t="s">
+        <v>12</v>
+      </c>
+      <c r="F974" t="s">
+        <v>12</v>
+      </c>
+      <c r="G974" t="s">
+        <v>12</v>
+      </c>
+      <c r="H974" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="975" spans="1:8">
+      <c r="A975" t="s">
+        <v>2926</v>
+      </c>
+      <c r="B975" t="s">
+        <v>14</v>
+      </c>
+      <c r="C975" t="s">
+        <v>2927</v>
+      </c>
+      <c r="D975" t="s">
+        <v>2928</v>
+      </c>
+      <c r="E975" t="s">
+        <v>23</v>
+      </c>
+      <c r="F975" t="s">
+        <v>23</v>
+      </c>
+      <c r="G975" t="s">
+        <v>23</v>
+      </c>
+      <c r="H975" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="976" spans="1:8">
+      <c r="A976" t="s">
+        <v>2929</v>
+      </c>
+      <c r="B976" t="s">
+        <v>14</v>
+      </c>
+      <c r="C976" t="s">
+        <v>2930</v>
+      </c>
+      <c r="D976" t="s">
+        <v>2931</v>
+      </c>
+      <c r="E976" t="s">
+        <v>12</v>
+      </c>
+      <c r="F976" t="s">
+        <v>12</v>
+      </c>
+      <c r="G976" t="s">
+        <v>12</v>
+      </c>
+      <c r="H976" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="977" spans="1:8">
+      <c r="A977" t="s">
+        <v>2932</v>
+      </c>
+      <c r="B977" t="s">
+        <v>9</v>
+      </c>
+      <c r="C977" t="s">
+        <v>2933</v>
+      </c>
+      <c r="D977" t="s">
+        <v>2934</v>
+      </c>
+      <c r="E977" t="s">
+        <v>12</v>
+      </c>
+      <c r="F977" t="s">
+        <v>12</v>
+      </c>
+      <c r="G977" t="s">
+        <v>12</v>
+      </c>
+      <c r="H977" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="978" spans="1:8">
+      <c r="A978" t="s">
+        <v>2935</v>
+      </c>
+      <c r="B978" t="s">
+        <v>9</v>
+      </c>
+      <c r="C978" t="s">
+        <v>2936</v>
+      </c>
+      <c r="D978" t="s">
+        <v>2937</v>
+      </c>
+      <c r="E978" t="s">
+        <v>12</v>
+      </c>
+      <c r="F978" t="s">
+        <v>12</v>
+      </c>
+      <c r="G978" t="s">
+        <v>12</v>
+      </c>
+      <c r="H978" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="979" spans="1:8">
+      <c r="A979" t="s">
+        <v>2938</v>
+      </c>
+      <c r="B979" t="s">
+        <v>14</v>
+      </c>
+      <c r="C979" t="s">
+        <v>2939</v>
+      </c>
+      <c r="D979" t="s">
+        <v>2940</v>
+      </c>
+      <c r="E979" t="s">
+        <v>12</v>
+      </c>
+      <c r="F979" t="s">
+        <v>12</v>
+      </c>
+      <c r="G979" t="s">
+        <v>12</v>
+      </c>
+      <c r="H979" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="980" spans="1:8">
+      <c r="A980" t="s">
+        <v>2941</v>
+      </c>
+      <c r="B980" t="s">
+        <v>9</v>
+      </c>
+      <c r="C980" t="s">
+        <v>2942</v>
+      </c>
+      <c r="D980" t="s">
+        <v>2943</v>
+      </c>
+      <c r="E980" t="s">
+        <v>23</v>
+      </c>
+      <c r="F980" t="s">
+        <v>23</v>
+      </c>
+      <c r="G980" t="s">
+        <v>23</v>
+      </c>
+      <c r="H980" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="981" spans="1:8">
+      <c r="A981" t="s">
+        <v>2944</v>
+      </c>
+      <c r="B981" t="s">
+        <v>9</v>
+      </c>
+      <c r="C981" t="s">
+        <v>2945</v>
+      </c>
+      <c r="D981" t="s">
+        <v>2946</v>
+      </c>
+      <c r="E981" t="s">
+        <v>12</v>
+      </c>
+      <c r="F981" t="s">
+        <v>12</v>
+      </c>
+      <c r="G981" t="s">
+        <v>12</v>
+      </c>
+      <c r="H981" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="982" spans="1:8">
+      <c r="A982" t="s">
+        <v>2947</v>
+      </c>
+      <c r="B982" t="s">
+        <v>9</v>
+      </c>
+      <c r="C982" t="s">
+        <v>2948</v>
+      </c>
+      <c r="D982" t="s">
+        <v>2949</v>
+      </c>
+      <c r="E982" t="s">
+        <v>12</v>
+      </c>
+      <c r="F982" t="s">
+        <v>23</v>
+      </c>
+      <c r="G982" t="s">
+        <v>12</v>
+      </c>
+      <c r="H982" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="983" spans="1:8">
+      <c r="A983" t="s">
+        <v>2950</v>
+      </c>
+      <c r="B983" t="s">
+        <v>9</v>
+      </c>
+      <c r="C983" t="s">
+        <v>2951</v>
+      </c>
+      <c r="D983" t="s">
+        <v>2952</v>
+      </c>
+      <c r="E983" t="s">
+        <v>12</v>
+      </c>
+      <c r="F983" t="s">
+        <v>12</v>
+      </c>
+      <c r="G983" t="s">
+        <v>12</v>
+      </c>
+      <c r="H983" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="984" spans="1:8">
+      <c r="A984" t="s">
+        <v>2953</v>
+      </c>
+      <c r="B984" t="s">
+        <v>14</v>
+      </c>
+      <c r="C984" t="s">
+        <v>2954</v>
+      </c>
+      <c r="D984" t="s">
+        <v>2955</v>
+      </c>
+      <c r="E984" t="s">
+        <v>12</v>
+      </c>
+      <c r="F984" t="s">
+        <v>12</v>
+      </c>
+      <c r="G984" t="s">
+        <v>12</v>
+      </c>
+      <c r="H984" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="985" spans="1:8">
+      <c r="A985" t="s">
+        <v>2956</v>
+      </c>
+      <c r="B985" t="s">
+        <v>9</v>
+      </c>
+      <c r="C985" t="s">
+        <v>2957</v>
+      </c>
+      <c r="D985" t="s">
+        <v>2958</v>
+      </c>
+      <c r="E985" t="s">
+        <v>12</v>
+      </c>
+      <c r="F985" t="s">
+        <v>12</v>
+      </c>
+      <c r="G985" t="s">
+        <v>12</v>
+      </c>
+      <c r="H985" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="986" spans="1:8">
+      <c r="A986" t="s">
+        <v>2959</v>
+      </c>
+      <c r="B986" t="s">
+        <v>9</v>
+      </c>
+      <c r="C986" t="s">
+        <v>2960</v>
+      </c>
+      <c r="D986" t="s">
+        <v>2961</v>
+      </c>
+      <c r="E986" t="s">
+        <v>12</v>
+      </c>
+      <c r="F986" t="s">
+        <v>12</v>
+      </c>
+      <c r="G986" t="s">
+        <v>12</v>
+      </c>
+      <c r="H986" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="987" spans="1:8">
+      <c r="A987" t="s">
+        <v>2962</v>
+      </c>
+      <c r="B987" t="s">
+        <v>14</v>
+      </c>
+      <c r="C987" t="s">
+        <v>2963</v>
+      </c>
+      <c r="D987" t="s">
+        <v>2964</v>
+      </c>
+      <c r="E987" t="s">
+        <v>12</v>
+      </c>
+      <c r="F987" t="s">
+        <v>12</v>
+      </c>
+      <c r="G987" t="s">
+        <v>12</v>
+      </c>
+      <c r="H987" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="988" spans="1:8">
+      <c r="A988" t="s">
+        <v>2965</v>
+      </c>
+      <c r="B988" t="s">
+        <v>9</v>
+      </c>
+      <c r="C988" t="s">
+        <v>2966</v>
+      </c>
+      <c r="D988" t="s">
+        <v>2967</v>
+      </c>
+      <c r="E988" t="s">
+        <v>12</v>
+      </c>
+      <c r="F988" t="s">
+        <v>12</v>
+      </c>
+      <c r="G988" t="s">
+        <v>12</v>
+      </c>
+      <c r="H988" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="989" spans="1:8">
+      <c r="A989" t="s">
+        <v>2968</v>
+      </c>
+      <c r="B989" t="s">
+        <v>14</v>
+      </c>
+      <c r="C989" t="s">
+        <v>2969</v>
+      </c>
+      <c r="D989" t="s">
+        <v>2970</v>
+      </c>
+      <c r="E989" t="s">
+        <v>12</v>
+      </c>
+      <c r="F989" t="s">
+        <v>12</v>
+      </c>
+      <c r="G989" t="s">
+        <v>12</v>
+      </c>
+      <c r="H989" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="990" spans="1:8">
+      <c r="A990" t="s">
+        <v>2971</v>
+      </c>
+      <c r="B990" t="s">
+        <v>14</v>
+      </c>
+      <c r="C990" t="s">
+        <v>2972</v>
+      </c>
+      <c r="D990" t="s">
+        <v>2973</v>
+      </c>
+      <c r="E990" t="s">
+        <v>12</v>
+      </c>
+      <c r="F990" t="s">
+        <v>12</v>
+      </c>
+      <c r="G990" t="s">
+        <v>12</v>
+      </c>
+      <c r="H990" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="991" spans="1:8">
+      <c r="A991" t="s">
+        <v>2974</v>
+      </c>
+      <c r="B991" t="s">
+        <v>14</v>
+      </c>
+      <c r="C991" t="s">
+        <v>2975</v>
+      </c>
+      <c r="D991" t="s">
+        <v>2976</v>
+      </c>
+      <c r="E991" t="s">
+        <v>12</v>
+      </c>
+      <c r="F991" t="s">
+        <v>12</v>
+      </c>
+      <c r="G991" t="s">
+        <v>12</v>
+      </c>
+      <c r="H991" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="992" spans="1:8">
+      <c r="A992" t="s">
+        <v>2977</v>
+      </c>
+      <c r="B992" t="s">
+        <v>9</v>
+      </c>
+      <c r="C992" t="s">
+        <v>2978</v>
+      </c>
+      <c r="D992" t="s">
+        <v>2979</v>
+      </c>
+      <c r="E992" t="s">
+        <v>23</v>
+      </c>
+      <c r="F992" t="s">
+        <v>23</v>
+      </c>
+      <c r="G992" t="s">
+        <v>23</v>
+      </c>
+      <c r="H992" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="993" spans="1:8">
+      <c r="A993" t="s">
+        <v>2980</v>
+      </c>
+      <c r="B993" t="s">
+        <v>9</v>
+      </c>
+      <c r="C993" t="s">
+        <v>2981</v>
+      </c>
+      <c r="D993" t="s">
+        <v>2982</v>
+      </c>
+      <c r="E993" t="s">
+        <v>12</v>
+      </c>
+      <c r="F993" t="s">
+        <v>12</v>
+      </c>
+      <c r="G993" t="s">
+        <v>12</v>
+      </c>
+      <c r="H993" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="994" spans="1:8">
+      <c r="A994" t="s">
+        <v>2983</v>
+      </c>
+      <c r="B994" t="s">
+        <v>9</v>
+      </c>
+      <c r="C994" t="s">
+        <v>2984</v>
+      </c>
+      <c r="D994" t="s">
+        <v>2985</v>
+      </c>
+      <c r="E994" t="s">
+        <v>12</v>
+      </c>
+      <c r="F994" t="s">
+        <v>12</v>
+      </c>
+      <c r="G994" t="s">
+        <v>12</v>
+      </c>
+      <c r="H994" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="995" spans="1:8">
+      <c r="A995" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B995" t="s">
+        <v>9</v>
+      </c>
+      <c r="C995" t="s">
+        <v>2987</v>
+      </c>
+      <c r="D995" t="s">
+        <v>2988</v>
+      </c>
+      <c r="E995" t="s">
+        <v>23</v>
+      </c>
+      <c r="F995" t="s">
+        <v>23</v>
+      </c>
+      <c r="G995" t="s">
+        <v>23</v>
+      </c>
+      <c r="H995" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="996" spans="1:8">
+      <c r="A996" t="s">
+        <v>2989</v>
+      </c>
+      <c r="B996" t="s">
+        <v>9</v>
+      </c>
+      <c r="C996" t="s">
+        <v>2990</v>
+      </c>
+      <c r="D996" t="s">
+        <v>2991</v>
+      </c>
+      <c r="E996" t="s">
+        <v>12</v>
+      </c>
+      <c r="F996" t="s">
+        <v>12</v>
+      </c>
+      <c r="G996" t="s">
+        <v>12</v>
+      </c>
+      <c r="H996" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="997" spans="1:8">
+      <c r="A997" t="s">
+        <v>2992</v>
+      </c>
+      <c r="B997" t="s">
+        <v>9</v>
+      </c>
+      <c r="C997" t="s">
+        <v>2993</v>
+      </c>
+      <c r="D997" t="s">
+        <v>2994</v>
+      </c>
+      <c r="E997" t="s">
+        <v>12</v>
+      </c>
+      <c r="F997" t="s">
+        <v>23</v>
+      </c>
+      <c r="G997" t="s">
+        <v>12</v>
+      </c>
+      <c r="H997" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="998" spans="1:8">
+      <c r="A998" t="s">
+        <v>2995</v>
+      </c>
+      <c r="B998" t="s">
+        <v>9</v>
+      </c>
+      <c r="C998" t="s">
+        <v>2996</v>
+      </c>
+      <c r="D998" t="s">
+        <v>2997</v>
+      </c>
+      <c r="E998" t="s">
+        <v>12</v>
+      </c>
+      <c r="F998" t="s">
+        <v>23</v>
+      </c>
+      <c r="G998" t="s">
+        <v>12</v>
+      </c>
+      <c r="H998" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="999" spans="1:8">
+      <c r="A999" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B999" t="s">
+        <v>9</v>
+      </c>
+      <c r="C999" t="s">
+        <v>2999</v>
+      </c>
+      <c r="D999" t="s">
+        <v>3000</v>
+      </c>
+      <c r="E999" t="s">
+        <v>23</v>
+      </c>
+      <c r="F999" t="s">
+        <v>23</v>
+      </c>
+      <c r="G999" t="s">
+        <v>23</v>
+      </c>
+      <c r="H999" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:8">
+      <c r="A1000" t="s">
+        <v>3001</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>3002</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>3003</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1000" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1000" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1000" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:8">
+      <c r="A1001" t="s">
+        <v>3004</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>3005</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>3006</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1001" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1001" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1001" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:8">
+      <c r="A1002" t="s">
+        <v>3007</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>3008</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>3009</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1002" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1002" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1002" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:8">
+      <c r="A1003" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>3011</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>3012</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1003" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1003" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:8">
+      <c r="A1004" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>3014</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>3015</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1004" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1004" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1004" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:8">
+      <c r="A1005" t="s">
+        <v>3016</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>3017</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>3018</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1005" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1005" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1005" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:8">
+      <c r="A1006" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>3020</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>3021</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1006" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1006" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1006" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:8">
+      <c r="A1007" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>3023</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>3024</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1007" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1007" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1007" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:8">
+      <c r="A1008" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>3026</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>3027</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1008" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1008" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1008" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:8">
+      <c r="A1009" t="s">
+        <v>3028</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>3029</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>3030</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1009" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1009" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1009" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:8">
+      <c r="A1010" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>3032</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>3033</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1010" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1010" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1010" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:8">
+      <c r="A1011" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>3035</v>
+      </c>
+      <c r="D1011" t="s">
+        <v>3036</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1011" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1011" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1011" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:8">
+      <c r="A1012" t="s">
+        <v>3037</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>3038</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>3039</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1012" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1012" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1012" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:8">
+      <c r="A1013" t="s">
+        <v>3040</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>3041</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>3042</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1013" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1013" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1013" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>